<commit_message>
Added start and end time stamps
</commit_message>
<xml_diff>
--- a/BME 355/Project/data/data.xlsx
+++ b/BME 355/Project/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\School\3A\BME 355\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grace\source\repos\Uni-Projects\BME 355\Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24DDB89-F7D3-42F3-BF27-772B6EDAABE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9D7826-78B8-4204-A8DC-A3778F1B393F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>time</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>Height Adjustment Factor</t>
+  </si>
+  <si>
+    <t>Start Time (s)</t>
+  </si>
+  <si>
+    <t>End Time (s)</t>
   </si>
 </sst>
 </file>
@@ -3461,15 +3467,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>212725</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>111125</xdr:rowOff>
+      <xdr:colOff>244475</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>92075</xdr:rowOff>
+      <xdr:colOff>727075</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3497,15 +3503,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3835,7 +3841,7 @@
   <dimension ref="A1:K74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4156,6 +4162,12 @@
         <f t="shared" si="1"/>
         <v>3.1148040156381285E-3</v>
       </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -4183,6 +4195,12 @@
       <c r="H11">
         <f t="shared" si="1"/>
         <v>4.2889845957959638E-3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11">
+        <v>1.35</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added formula to calculate distance between ankle joint and balls of the feet
</commit_message>
<xml_diff>
--- a/BME 355/Project/data/data.xlsx
+++ b/BME 355/Project/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grace\source\repos\Uni-Projects\BME 355\Project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Uni-Projects\BME 355\Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9D7826-78B8-4204-A8DC-A3778F1B393F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13194040-8A01-4394-A19E-355AB1596F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>time</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>End Time (s)</t>
+  </si>
+  <si>
+    <t>Foot Length (m)</t>
   </si>
 </sst>
 </file>
@@ -3841,7 +3844,8 @@
   <dimension ref="A1:K74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3871,12 +3875,6 @@
       <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1">
-        <v>0.1950308</v>
-      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -3902,14 +3900,14 @@
         <v>8.3134362900000003</v>
       </c>
       <c r="H2">
-        <f>B2-$K$5*COS(RADIANS(C2+D2))-$K$6*COS(RADIANS(C2+D2+E2))-$K$8</f>
+        <f>B2-$K$6*COS(RADIANS(C2+D2))-$K$7*COS(RADIANS(C2+D2+E2))-$K$10</f>
         <v>7.116865845925302E-4</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>0.18455724409999999</v>
+        <v>0.1950308</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -3936,15 +3934,14 @@
         <v>8.8110470799999998</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H66" si="1">B3-$K$5*COS(RADIANS(C3+D3))-$K$6*COS(RADIANS(C3+D3+E3))-$K$8</f>
+        <f>B3-$K$6*COS(RADIANS(C3+D3))-$K$7*COS(RADIANS(C3+D3+E3))-$K$10</f>
         <v>9.1260743201959649E-4</v>
       </c>
       <c r="J3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3">
-        <f>1.045</f>
-        <v>1.0449999999999999</v>
+        <v>0.18455724409999999</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -3971,8 +3968,15 @@
         <v>9.3249314499999993</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f>B4-$K$6*COS(RADIANS(C4+D4))-$K$7*COS(RADIANS(C4+D4+E4))-$K$10</f>
         <v>8.6453401385977457E-4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <f>1.045</f>
+        <v>1.0449999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -3999,15 +4003,8 @@
         <v>9.9451065000000014</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f>B5-$K$6*COS(RADIANS(C5+D5))-$K$7*COS(RADIANS(C5+D5+E5))-$K$10</f>
         <v>1.1958020955685766E-3</v>
-      </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5">
-        <f>K1/(K1+K2)*K3</f>
-        <v>0.53691676850156089</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -4034,15 +4031,15 @@
         <v>10.63320731</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f>B6-$K$6*COS(RADIANS(C6+D6))-$K$7*COS(RADIANS(C6+D6+E6))-$K$10</f>
         <v>1.0083137324033431E-3</v>
       </c>
       <c r="J6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K6">
-        <f>K2/(K1+K2)*K3</f>
-        <v>0.50808323149843904</v>
+        <f>K2/(K2+K3)*K4</f>
+        <v>0.53691676850156089</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -4069,8 +4066,15 @@
         <v>11.26421538</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f>B7-$K$6*COS(RADIANS(C7+D7))-$K$7*COS(RADIANS(C7+D7+E7))-$K$10</f>
         <v>1.5440728229624834E-3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <f>K3/(K2+K3)*K4</f>
+        <v>0.50808323149843904</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -4097,14 +4101,15 @@
         <v>11.95883149</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f>B8-$K$6*COS(RADIANS(C8+D8))-$K$7*COS(RADIANS(C8+D8+E8))-$K$10</f>
         <v>2.049032133853157E-3</v>
       </c>
       <c r="J8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K8">
-        <v>4.7697474025435449E-3</v>
+        <f>-H23/SIN(RADIANS(F23-G23))</f>
+        <v>0.18492841020407733</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -4131,7 +4136,7 @@
         <v>12.771557440000002</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f>B9-$K$6*COS(RADIANS(C9+D9))-$K$7*COS(RADIANS(C9+D9+E9))-$K$10</f>
         <v>2.5035843062888308E-3</v>
       </c>
     </row>
@@ -4159,14 +4164,14 @@
         <v>13.748658259999999</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f>B10-$K$6*COS(RADIANS(C10+D10))-$K$7*COS(RADIANS(C10+D10+E10))-$K$10</f>
         <v>3.1148040156381285E-3</v>
       </c>
       <c r="J10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K10">
-        <v>0.75</v>
+        <v>4.7697474025435449E-3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -4193,14 +4198,8 @@
         <v>14.740358460000001</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f>B11-$K$6*COS(RADIANS(C11+D11))-$K$7*COS(RADIANS(C11+D11+E11))-$K$10</f>
         <v>4.2889845957959638E-3</v>
-      </c>
-      <c r="J11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11">
-        <v>1.35</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -4227,8 +4226,14 @@
         <v>15.935775869999999</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f>B12-$K$6*COS(RADIANS(C12+D12))-$K$7*COS(RADIANS(C12+D12+E12))-$K$10</f>
         <v>5.9003631058472394E-3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12">
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -4255,8 +4260,14 @@
         <v>17.504851719999998</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
+        <f>B13-$K$6*COS(RADIANS(C13+D13))-$K$7*COS(RADIANS(C13+D13+E13))-$K$10</f>
         <v>8.1924473549296883E-3</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13">
+        <v>1.35</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -4283,7 +4294,7 @@
         <v>19.06587863</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
+        <f>B14-$K$6*COS(RADIANS(C14+D14))-$K$7*COS(RADIANS(C14+D14+E14))-$K$10</f>
         <v>1.2297223767784748E-2</v>
       </c>
     </row>
@@ -4311,7 +4322,7 @@
         <v>20.908707190000001</v>
       </c>
       <c r="H15">
-        <f t="shared" si="1"/>
+        <f>B15-$K$6*COS(RADIANS(C15+D15))-$K$7*COS(RADIANS(C15+D15+E15))-$K$10</f>
         <v>1.7191415794078901E-2</v>
       </c>
     </row>
@@ -4339,7 +4350,7 @@
         <v>22.901764400000001</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
+        <f>B16-$K$6*COS(RADIANS(C16+D16))-$K$7*COS(RADIANS(C16+D16+E16))-$K$10</f>
         <v>2.3410577379752273E-2</v>
       </c>
     </row>
@@ -4367,7 +4378,7 @@
         <v>24.992742509999999</v>
       </c>
       <c r="H17">
-        <f t="shared" si="1"/>
+        <f>B17-$K$6*COS(RADIANS(C17+D17))-$K$7*COS(RADIANS(C17+D17+E17))-$K$10</f>
         <v>3.0533244046068053E-2</v>
       </c>
     </row>
@@ -4395,7 +4406,7 @@
         <v>27.292966329999999</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
+        <f>B18-$K$6*COS(RADIANS(C18+D18))-$K$7*COS(RADIANS(C18+D18+E18))-$K$10</f>
         <v>3.9180989531838406E-2</v>
       </c>
     </row>
@@ -4423,7 +4434,7 @@
         <v>29.900414099999999</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
+        <f>B19-$K$6*COS(RADIANS(C19+D19))-$K$7*COS(RADIANS(C19+D19+E19))-$K$10</f>
         <v>4.9623117916908099E-2</v>
       </c>
     </row>
@@ -4451,7 +4462,7 @@
         <v>32.820760409999998</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
+        <f>B20-$K$6*COS(RADIANS(C20+D20))-$K$7*COS(RADIANS(C20+D20+E20))-$K$10</f>
         <v>6.2844480971263939E-2</v>
       </c>
     </row>
@@ -4479,7 +4490,7 @@
         <v>36.11288571</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
+        <f>B21-$K$6*COS(RADIANS(C21+D21))-$K$7*COS(RADIANS(C21+D21+E21))-$K$10</f>
         <v>7.8032151444156983E-2</v>
       </c>
     </row>
@@ -4507,7 +4518,7 @@
         <v>39.965340939999997</v>
       </c>
       <c r="H22">
-        <f t="shared" si="1"/>
+        <f>B22-$K$6*COS(RADIANS(C22+D22))-$K$7*COS(RADIANS(C22+D22+E22))-$K$10</f>
         <v>9.5443317830569585E-2</v>
       </c>
     </row>
@@ -4535,7 +4546,7 @@
         <v>43.748470879999999</v>
       </c>
       <c r="H23">
-        <f t="shared" si="1"/>
+        <f>B23-$K$6*COS(RADIANS(C23+D23))-$K$7*COS(RADIANS(C23+D23+E23))-$K$10</f>
         <v>0.1145101481908945</v>
       </c>
     </row>
@@ -4563,7 +4574,7 @@
         <v>47.387127019999994</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
+        <f>B24-$K$6*COS(RADIANS(C24+D24))-$K$7*COS(RADIANS(C24+D24+E24))-$K$10</f>
         <v>0.13423640324778313</v>
       </c>
     </row>
@@ -4591,7 +4602,7 @@
         <v>50.523246079999993</v>
       </c>
       <c r="H25">
-        <f t="shared" si="1"/>
+        <f>B25-$K$6*COS(RADIANS(C25+D25))-$K$7*COS(RADIANS(C25+D25+E25))-$K$10</f>
         <v>0.15323679456369976</v>
       </c>
     </row>
@@ -4619,7 +4630,7 @@
         <v>53.131709280000003</v>
       </c>
       <c r="H26">
-        <f t="shared" si="1"/>
+        <f>B26-$K$6*COS(RADIANS(C26+D26))-$K$7*COS(RADIANS(C26+D26+E26))-$K$10</f>
         <v>0.17130633826703734</v>
       </c>
     </row>
@@ -4647,7 +4658,7 @@
         <v>55.025795870000003</v>
       </c>
       <c r="H27">
-        <f t="shared" si="1"/>
+        <f>B27-$K$6*COS(RADIANS(C27+D27))-$K$7*COS(RADIANS(C27+D27+E27))-$K$10</f>
         <v>0.18718269341486676</v>
       </c>
     </row>
@@ -4675,7 +4686,7 @@
         <v>56.293017239999998</v>
       </c>
       <c r="H28">
-        <f t="shared" si="1"/>
+        <f>B28-$K$6*COS(RADIANS(C28+D28))-$K$7*COS(RADIANS(C28+D28+E28))-$K$10</f>
         <v>0.20054261109685689</v>
       </c>
     </row>
@@ -4703,7 +4714,7 @@
         <v>56.937211310000002</v>
       </c>
       <c r="H29">
-        <f t="shared" si="1"/>
+        <f>B29-$K$6*COS(RADIANS(C29+D29))-$K$7*COS(RADIANS(C29+D29+E29))-$K$10</f>
         <v>0.21090315205236621</v>
       </c>
     </row>
@@ -4731,7 +4742,7 @@
         <v>56.892690770000002</v>
       </c>
       <c r="H30">
-        <f t="shared" si="1"/>
+        <f>B30-$K$6*COS(RADIANS(C30+D30))-$K$7*COS(RADIANS(C30+D30+E30))-$K$10</f>
         <v>0.2172766258325512</v>
       </c>
     </row>
@@ -4759,7 +4770,7 @@
         <v>56.117676069999995</v>
       </c>
       <c r="H31">
-        <f t="shared" si="1"/>
+        <f>B31-$K$6*COS(RADIANS(C31+D31))-$K$7*COS(RADIANS(C31+D31+E31))-$K$10</f>
         <v>0.21904796091100515</v>
       </c>
     </row>
@@ -4787,7 +4798,7 @@
         <v>54.731604529999998</v>
       </c>
       <c r="H32">
-        <f t="shared" si="1"/>
+        <f>B32-$K$6*COS(RADIANS(C32+D32))-$K$7*COS(RADIANS(C32+D32+E32))-$K$10</f>
         <v>0.21682194449721637</v>
       </c>
     </row>
@@ -4815,7 +4826,7 @@
         <v>52.653334729999997</v>
       </c>
       <c r="H33">
-        <f t="shared" si="1"/>
+        <f>B33-$K$6*COS(RADIANS(C33+D33))-$K$7*COS(RADIANS(C33+D33+E33))-$K$10</f>
         <v>0.20988608432065931</v>
       </c>
     </row>
@@ -4843,7 +4854,7 @@
         <v>49.958357570000004</v>
       </c>
       <c r="H34">
-        <f t="shared" si="1"/>
+        <f>B34-$K$6*COS(RADIANS(C34+D34))-$K$7*COS(RADIANS(C34+D34+E34))-$K$10</f>
         <v>0.19892088731401653</v>
       </c>
     </row>
@@ -4871,7 +4882,7 @@
         <v>46.733945739999996</v>
       </c>
       <c r="H35">
-        <f t="shared" si="1"/>
+        <f>B35-$K$6*COS(RADIANS(C35+D35))-$K$7*COS(RADIANS(C35+D35+E35))-$K$10</f>
         <v>0.18411312598422808</v>
       </c>
     </row>
@@ -4899,7 +4910,7 @@
         <v>42.980657910000005</v>
       </c>
       <c r="H36">
-        <f t="shared" si="1"/>
+        <f>B36-$K$6*COS(RADIANS(C36+D36))-$K$7*COS(RADIANS(C36+D36+E36))-$K$10</f>
         <v>0.1667741547718396</v>
       </c>
     </row>
@@ -4927,7 +4938,7 @@
         <v>38.835042449999996</v>
       </c>
       <c r="H37">
-        <f t="shared" si="1"/>
+        <f>B37-$K$6*COS(RADIANS(C37+D37))-$K$7*COS(RADIANS(C37+D37+E37))-$K$10</f>
         <v>0.14779077984641925</v>
       </c>
     </row>
@@ -4955,7 +4966,7 @@
         <v>34.149562549999999</v>
       </c>
       <c r="H38">
-        <f t="shared" si="1"/>
+        <f>B38-$K$6*COS(RADIANS(C38+D38))-$K$7*COS(RADIANS(C38+D38+E38))-$K$10</f>
         <v>0.12739154148061121</v>
       </c>
     </row>
@@ -4983,7 +4994,7 @@
         <v>29.146503530000004</v>
       </c>
       <c r="H39">
-        <f t="shared" si="1"/>
+        <f>B39-$K$6*COS(RADIANS(C39+D39))-$K$7*COS(RADIANS(C39+D39+E39))-$K$10</f>
         <v>0.10688229884476697</v>
       </c>
     </row>
@@ -5011,7 +5022,7 @@
         <v>23.84913392</v>
       </c>
       <c r="H40">
-        <f t="shared" si="1"/>
+        <f>B40-$K$6*COS(RADIANS(C40+D40))-$K$7*COS(RADIANS(C40+D40+E40))-$K$10</f>
         <v>8.7505283312476922E-2</v>
       </c>
     </row>
@@ -5039,7 +5050,7 @@
         <v>18.289900220000003</v>
       </c>
       <c r="H41">
-        <f t="shared" si="1"/>
+        <f>B41-$K$6*COS(RADIANS(C41+D41))-$K$7*COS(RADIANS(C41+D41+E41))-$K$10</f>
         <v>7.025016139349255E-2</v>
       </c>
     </row>
@@ -5067,7 +5078,7 @@
         <v>12.638638090000001</v>
       </c>
       <c r="H42">
-        <f t="shared" si="1"/>
+        <f>B42-$K$6*COS(RADIANS(C42+D42))-$K$7*COS(RADIANS(C42+D42+E42))-$K$10</f>
         <v>5.5769063846833278E-2</v>
       </c>
     </row>
@@ -5095,7 +5106,7 @@
         <v>6.8685695899999999</v>
       </c>
       <c r="H43">
-        <f t="shared" si="1"/>
+        <f>B43-$K$6*COS(RADIANS(C43+D43))-$K$7*COS(RADIANS(C43+D43+E43))-$K$10</f>
         <v>4.4631769934232235E-2</v>
       </c>
     </row>
@@ -5123,7 +5134,7 @@
         <v>1.2876091899999977</v>
       </c>
       <c r="H44">
-        <f t="shared" si="1"/>
+        <f>B44-$K$6*COS(RADIANS(C44+D44))-$K$7*COS(RADIANS(C44+D44+E44))-$K$10</f>
         <v>3.8066434157436269E-2</v>
       </c>
     </row>
@@ -5151,7 +5162,7 @@
         <v>-4.2347093099999995</v>
       </c>
       <c r="H45">
-        <f t="shared" si="1"/>
+        <f>B45-$K$6*COS(RADIANS(C45+D45))-$K$7*COS(RADIANS(C45+D45+E45))-$K$10</f>
         <v>3.5350444430718553E-2</v>
       </c>
     </row>
@@ -5179,7 +5190,7 @@
         <v>-9.3443700599999993</v>
       </c>
       <c r="H46">
-        <f t="shared" si="1"/>
+        <f>B46-$K$6*COS(RADIANS(C46+D46))-$K$7*COS(RADIANS(C46+D46+E46))-$K$10</f>
         <v>3.6476976040728082E-2</v>
       </c>
     </row>
@@ -5207,7 +5218,7 @@
         <v>-14.055747479999999</v>
       </c>
       <c r="H47">
-        <f t="shared" si="1"/>
+        <f>B47-$K$6*COS(RADIANS(C47+D47))-$K$7*COS(RADIANS(C47+D47+E47))-$K$10</f>
         <v>4.020957671277603E-2</v>
       </c>
     </row>
@@ -5235,7 +5246,7 @@
         <v>-17.876357980000002</v>
       </c>
       <c r="H48">
-        <f t="shared" si="1"/>
+        <f>B48-$K$6*COS(RADIANS(C48+D48))-$K$7*COS(RADIANS(C48+D48+E48))-$K$10</f>
         <v>4.4721659343532505E-2</v>
       </c>
     </row>
@@ -5263,7 +5274,7 @@
         <v>-20.644239709999997</v>
       </c>
       <c r="H49">
-        <f t="shared" si="1"/>
+        <f>B49-$K$6*COS(RADIANS(C49+D49))-$K$7*COS(RADIANS(C49+D49+E49))-$K$10</f>
         <v>4.8687397744538286E-2</v>
       </c>
     </row>
@@ -5291,7 +5302,7 @@
         <v>-22.326335380000003</v>
       </c>
       <c r="H50">
-        <f t="shared" si="1"/>
+        <f>B50-$K$6*COS(RADIANS(C50+D50))-$K$7*COS(RADIANS(C50+D50+E50))-$K$10</f>
         <v>5.0434615952563155E-2</v>
       </c>
     </row>
@@ -5319,7 +5330,7 @@
         <v>-22.654323860000002</v>
       </c>
       <c r="H51">
-        <f t="shared" si="1"/>
+        <f>B51-$K$6*COS(RADIANS(C51+D51))-$K$7*COS(RADIANS(C51+D51+E51))-$K$10</f>
         <v>5.001448083657245E-2</v>
       </c>
     </row>
@@ -5347,7 +5358,7 @@
         <v>-21.890587190000002</v>
       </c>
       <c r="H52">
-        <f t="shared" si="1"/>
+        <f>B52-$K$6*COS(RADIANS(C52+D52))-$K$7*COS(RADIANS(C52+D52+E52))-$K$10</f>
         <v>4.6484928838822326E-2</v>
       </c>
     </row>
@@ -5375,7 +5386,7 @@
         <v>-20.219596510000002</v>
       </c>
       <c r="H53">
-        <f t="shared" si="1"/>
+        <f>B53-$K$6*COS(RADIANS(C53+D53))-$K$7*COS(RADIANS(C53+D53+E53))-$K$10</f>
         <v>4.049533381557141E-2</v>
       </c>
     </row>
@@ -5403,7 +5414,7 @@
         <v>-18.054217040000001</v>
       </c>
       <c r="H54">
-        <f t="shared" si="1"/>
+        <f>B54-$K$6*COS(RADIANS(C54+D54))-$K$7*COS(RADIANS(C54+D54+E54))-$K$10</f>
         <v>3.4418892845651861E-2</v>
       </c>
     </row>
@@ -5431,7 +5442,7 @@
         <v>-15.831136979999998</v>
       </c>
       <c r="H55">
-        <f t="shared" si="1"/>
+        <f>B55-$K$6*COS(RADIANS(C55+D55))-$K$7*COS(RADIANS(C55+D55+E55))-$K$10</f>
         <v>2.904018514359763E-2</v>
       </c>
     </row>
@@ -5459,7 +5470,7 @@
         <v>-13.416914530000003</v>
       </c>
       <c r="H56">
-        <f t="shared" si="1"/>
+        <f>B56-$K$6*COS(RADIANS(C56+D56))-$K$7*COS(RADIANS(C56+D56+E56))-$K$10</f>
         <v>2.4333977182246169E-2</v>
       </c>
     </row>
@@ -5487,7 +5498,7 @@
         <v>-11.027822700000002</v>
       </c>
       <c r="H57">
-        <f t="shared" si="1"/>
+        <f>B57-$K$6*COS(RADIANS(C57+D57))-$K$7*COS(RADIANS(C57+D57+E57))-$K$10</f>
         <v>2.0673792478827779E-2</v>
       </c>
     </row>
@@ -5515,7 +5526,7 @@
         <v>-8.7046209199999982</v>
       </c>
       <c r="H58">
-        <f t="shared" si="1"/>
+        <f>B58-$K$6*COS(RADIANS(C58+D58))-$K$7*COS(RADIANS(C58+D58+E58))-$K$10</f>
         <v>1.782202706937297E-2</v>
       </c>
     </row>
@@ -5543,7 +5554,7 @@
         <v>-6.5187283899999997</v>
       </c>
       <c r="H59">
-        <f t="shared" si="1"/>
+        <f>B59-$K$6*COS(RADIANS(C59+D59))-$K$7*COS(RADIANS(C59+D59+E59))-$K$10</f>
         <v>1.5696353336845714E-2</v>
       </c>
     </row>
@@ -5571,7 +5582,7 @@
         <v>-4.5612783699999966</v>
       </c>
       <c r="H60">
-        <f t="shared" si="1"/>
+        <f>B60-$K$6*COS(RADIANS(C60+D60))-$K$7*COS(RADIANS(C60+D60+E60))-$K$10</f>
         <v>1.3615659272167902E-2</v>
       </c>
     </row>
@@ -5599,7 +5610,7 @@
         <v>-2.8798347700000022</v>
       </c>
       <c r="H61">
-        <f t="shared" si="1"/>
+        <f>B61-$K$6*COS(RADIANS(C61+D61))-$K$7*COS(RADIANS(C61+D61+E61))-$K$10</f>
         <v>1.1261997948185831E-2</v>
       </c>
     </row>
@@ -5627,7 +5638,7 @@
         <v>-1.3462972099999995</v>
       </c>
       <c r="H62">
-        <f t="shared" si="1"/>
+        <f>B62-$K$6*COS(RADIANS(C62+D62))-$K$7*COS(RADIANS(C62+D62+E62))-$K$10</f>
         <v>9.1062699711585982E-3</v>
       </c>
     </row>
@@ -5655,7 +5666,7 @@
         <v>-0.17492614000000017</v>
       </c>
       <c r="H63">
-        <f t="shared" si="1"/>
+        <f>B63-$K$6*COS(RADIANS(C63+D63))-$K$7*COS(RADIANS(C63+D63+E63))-$K$10</f>
         <v>6.9456642771068555E-3</v>
       </c>
     </row>
@@ -5683,7 +5694,7 @@
         <v>0.77253550000000004</v>
       </c>
       <c r="H64">
-        <f t="shared" si="1"/>
+        <f>B64-$K$6*COS(RADIANS(C64+D64))-$K$7*COS(RADIANS(C64+D64+E64))-$K$10</f>
         <v>4.8394325101331903E-3</v>
       </c>
     </row>
@@ -5711,7 +5722,7 @@
         <v>1.6695504699999972</v>
       </c>
       <c r="H65">
-        <f t="shared" si="1"/>
+        <f>B65-$K$6*COS(RADIANS(C65+D65))-$K$7*COS(RADIANS(C65+D65+E65))-$K$10</f>
         <v>3.39473300210269E-3</v>
       </c>
     </row>
@@ -5739,7 +5750,7 @@
         <v>2.5188072699999999</v>
       </c>
       <c r="H66">
-        <f t="shared" si="1"/>
+        <f>B66-$K$6*COS(RADIANS(C66+D66))-$K$7*COS(RADIANS(C66+D66+E66))-$K$10</f>
         <v>2.6195836683922114E-3</v>
       </c>
     </row>
@@ -5763,11 +5774,11 @@
         <v>1.9925147599999999</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G74" si="2">-C67-D67-E67</f>
+        <f t="shared" ref="G67:G74" si="1">-C67-D67-E67</f>
         <v>3.116057480000002</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H74" si="3">B67-$K$5*COS(RADIANS(C67+D67))-$K$6*COS(RADIANS(C67+D67+E67))-$K$8</f>
+        <f>B67-$K$6*COS(RADIANS(C67+D67))-$K$7*COS(RADIANS(C67+D67+E67))-$K$10</f>
         <v>2.0220618820427916E-3</v>
       </c>
     </row>
@@ -5791,11 +5802,11 @@
         <v>2.5513556799999999</v>
       </c>
       <c r="G68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.8097452300000008</v>
       </c>
       <c r="H68">
-        <f t="shared" si="3"/>
+        <f>B68-$K$6*COS(RADIANS(C68+D68))-$K$7*COS(RADIANS(C68+D68+E68))-$K$10</f>
         <v>1.6709306523434719E-3</v>
       </c>
     </row>
@@ -5819,11 +5830,11 @@
         <v>2.9746337899999999</v>
       </c>
       <c r="G69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.3368886799999995</v>
       </c>
       <c r="H69">
-        <f t="shared" si="3"/>
+        <f>B69-$K$6*COS(RADIANS(C69+D69))-$K$7*COS(RADIANS(C69+D69+E69))-$K$10</f>
         <v>1.3549758566331338E-3</v>
       </c>
     </row>
@@ -5847,11 +5858,11 @@
         <v>3.3282863699999998</v>
       </c>
       <c r="G70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.78943355</v>
       </c>
       <c r="H70">
-        <f t="shared" si="3"/>
+        <f>B70-$K$6*COS(RADIANS(C70+D70))-$K$7*COS(RADIANS(C70+D70+E70))-$K$10</f>
         <v>1.0495893530064748E-3</v>
       </c>
     </row>
@@ -5875,11 +5886,11 @@
         <v>3.7398007299999998</v>
       </c>
       <c r="G71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.3086282899999997</v>
       </c>
       <c r="H71">
-        <f t="shared" si="3"/>
+        <f>B71-$K$6*COS(RADIANS(C71+D71))-$K$7*COS(RADIANS(C71+D71+E71))-$K$10</f>
         <v>4.2587856066123031E-4</v>
       </c>
     </row>
@@ -5903,11 +5914,11 @@
         <v>4.1774215000000003</v>
       </c>
       <c r="G72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.8246162299999993</v>
       </c>
       <c r="H72">
-        <f t="shared" si="3"/>
+        <f>B72-$K$6*COS(RADIANS(C72+D72))-$K$7*COS(RADIANS(C72+D72+E72))-$K$10</f>
         <v>3.872033836704869E-4</v>
       </c>
     </row>
@@ -5931,11 +5942,11 @@
         <v>4.6742666100000001</v>
       </c>
       <c r="G73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.4111306599999995</v>
       </c>
       <c r="H73">
-        <f t="shared" si="3"/>
+        <f>B73-$K$6*COS(RADIANS(C73+D73))-$K$7*COS(RADIANS(C73+D73+E73))-$K$10</f>
         <v>2.1299940437380371E-4</v>
       </c>
     </row>
@@ -5959,11 +5970,11 @@
         <v>5.0655643799999996</v>
       </c>
       <c r="G74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.8754240399999986</v>
       </c>
       <c r="H74">
-        <f t="shared" si="3"/>
+        <f>B74-$K$6*COS(RADIANS(C74+D74))-$K$7*COS(RADIANS(C74+D74+E74))-$K$10</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
converted angles to radians
</commit_message>
<xml_diff>
--- a/BME 355/Project/data/data.xlsx
+++ b/BME 355/Project/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grace\source\repos\Uni-Projects\BME 355\Project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Uni-Projects\BME 355\Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCA5A0A-44EE-479C-AD5F-EE93DEF6DB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79102C80-11A5-4847-A03E-DBC635180865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1009,223 +1009,223 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="73"/>
                 <c:pt idx="0">
-                  <c:v>8.3134362900000003</c:v>
+                  <c:v>0.14509683541528215</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.8110470799999998</c:v>
+                  <c:v>0.15378178209423221</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.3249314499999993</c:v>
+                  <c:v>0.16275075632526897</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.9451065000000014</c:v>
+                  <c:v>0.17357485288648947</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.63320731</c:v>
+                  <c:v>0.18558447760662936</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.26421538</c:v>
+                  <c:v>0.19659764603478422</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.95883149</c:v>
+                  <c:v>0.20872098419167934</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.771557440000002</c:v>
+                  <c:v>0.22290572793557817</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.748658259999999</c:v>
+                  <c:v>0.23995935436851457</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.740358460000001</c:v>
+                  <c:v>0.25726778805120093</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.935775869999999</c:v>
+                  <c:v>0.27813175779136384</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17.504851719999998</c:v>
+                  <c:v>0.30551729758739249</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.06587863</c:v>
+                  <c:v>0.3327623568791257</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.908707190000001</c:v>
+                  <c:v>0.36492578280091165</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.901764400000001</c:v>
+                  <c:v>0.39971119329602367</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.992742509999999</c:v>
+                  <c:v>0.43620564590265176</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>27.292966329999999</c:v>
+                  <c:v>0.47635212509445313</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.900414099999999</c:v>
+                  <c:v>0.52186067375473699</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>32.820760409999998</c:v>
+                  <c:v>0.57283033216270407</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36.11288571</c:v>
+                  <c:v>0.63028875803591011</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>39.965340939999997</c:v>
+                  <c:v>0.69752678608508545</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43.748470879999999</c:v>
+                  <c:v>0.76355485956886104</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>47.387127019999994</c:v>
+                  <c:v>0.82706138955976882</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>50.523246079999993</c:v>
+                  <c:v>0.88179699289131819</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>53.131709280000003</c:v>
+                  <c:v>0.92732326414842581</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>55.025795870000003</c:v>
+                  <c:v>0.96038131146179773</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>56.293017239999998</c:v>
+                  <c:v>0.98249849671993095</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>56.937211310000002</c:v>
+                  <c:v>0.99374180426325387</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>56.892690770000002</c:v>
+                  <c:v>0.9929647742554879</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>56.117676069999995</c:v>
+                  <c:v>0.97943821598913172</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>54.731604529999998</c:v>
+                  <c:v>0.95524670394794353</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>52.653334729999997</c:v>
+                  <c:v>0.91897405319317937</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>49.958357570000004</c:v>
+                  <c:v>0.87193782848513357</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>46.733945739999996</c:v>
+                  <c:v>0.81566122561137777</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>42.980657910000005</c:v>
+                  <c:v>0.75015399520284476</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>38.835042449999996</c:v>
+                  <c:v>0.67779935590426521</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>34.149562549999999</c:v>
+                  <c:v>0.59602230461325068</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>29.146503530000004</c:v>
+                  <c:v>0.50870245204264997</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>23.84913392</c:v>
+                  <c:v>0.41624591065306188</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>18.289900220000003</c:v>
+                  <c:v>0.31921897870023525</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>12.638638090000001</c:v>
+                  <c:v>0.22058584763846742</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>6.8685695899999999</c:v>
+                  <c:v>0.11987915424785699</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.2876091899999977</c:v>
+                  <c:v>2.2473019844437205E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-4.2347093099999995</c:v>
+                  <c:v>-7.3909620324357217E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-9.3443700599999993</c:v>
+                  <c:v>-0.16309002407178005</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-14.055747479999999</c:v>
+                  <c:v>-0.24531907235489581</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-17.876357980000002</c:v>
+                  <c:v>-0.31200130501616263</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-20.644239709999997</c:v>
+                  <c:v>-0.36030995451045933</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-22.326335380000003</c:v>
+                  <c:v>-0.38966806228549938</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-22.654323860000002</c:v>
+                  <c:v>-0.39539254117011097</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-21.890587190000002</c:v>
+                  <c:v>-0.38206282166039351</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-20.219596510000002</c:v>
+                  <c:v>-0.35289853252425457</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-18.054217040000001</c:v>
+                  <c:v>-0.31510553121766477</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-15.831136979999998</c:v>
+                  <c:v>-0.27630546463523165</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-13.416914530000003</c:v>
+                  <c:v>-0.23416933400716755</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-11.027822700000002</c:v>
+                  <c:v>-0.1924718154411709</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-8.7046209199999982</c:v>
+                  <c:v>-0.15192429519197789</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-6.5187283899999997</c:v>
+                  <c:v>-0.11377327344872898</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-4.5612783699999966</c:v>
+                  <c:v>-7.9609325656500085E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-2.8798347700000022</c:v>
+                  <c:v>-5.0262598649913663E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-1.3462972099999995</c:v>
+                  <c:v>-2.3497319024913518E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-0.17492614000000017</c:v>
+                  <c:v>-3.0530370908045568E-3</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.77253550000000004</c:v>
+                  <c:v>1.3483288063540655E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.6695504699999972</c:v>
+                  <c:v>2.9139152729718763E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2.5188072699999999</c:v>
+                  <c:v>4.3961480084669789E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>3.116057480000002</c:v>
+                  <c:v>5.4385462707397393E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>3.8097452300000008</c:v>
+                  <c:v>6.6492597925648669E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4.3368886799999995</c:v>
+                  <c:v>7.5692986758470748E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4.78943355</c:v>
+                  <c:v>8.359138475298046E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5.3086282899999997</c:v>
+                  <c:v>9.265304242501636E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.8246162299999993</c:v>
+                  <c:v>0.10165873087859929</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>6.4111306599999995</c:v>
+                  <c:v>0.1118953387925571</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>6.8754240399999986</c:v>
+                  <c:v>0.1199987869687703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1926,7 +1926,7 @@
                   <c:v>4.9623117916908099E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.2844480971263939E-2</c:v>
+                  <c:v>6.2844480971263994E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>7.8032151444156983E-2</c:v>
@@ -1950,25 +1950,25 @@
                   <c:v>0.18718269341486676</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.20054261109685689</c:v>
+                  <c:v>0.20054261109685678</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.21090315205236621</c:v>
+                  <c:v>0.21090315205236626</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0.2172766258325512</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.21904796091100515</c:v>
+                  <c:v>0.2190479609110052</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.21682194449721637</c:v>
+                  <c:v>0.21682194449721626</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.20988608432065931</c:v>
+                  <c:v>0.20988608432065936</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.19892088731401653</c:v>
+                  <c:v>0.19892088731401658</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0.18411312598422808</c:v>
@@ -1977,13 +1977,13 @@
                   <c:v>0.1667741547718396</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.14779077984641925</c:v>
+                  <c:v>0.1477907798464192</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.12739154148061121</c:v>
+                  <c:v>0.12739154148061127</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.10688229884476697</c:v>
+                  <c:v>0.10688229884476691</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>8.7505283312476922E-2</c:v>
@@ -1992,7 +1992,7 @@
                   <c:v>7.025016139349255E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.5769063846833278E-2</c:v>
+                  <c:v>5.5769063846833167E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>4.4631769934232235E-2</c:v>
@@ -2010,7 +2010,7 @@
                   <c:v>4.020957671277603E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.4721659343532505E-2</c:v>
+                  <c:v>4.4721659343532338E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>4.8687397744538286E-2</c:v>
@@ -2019,7 +2019,7 @@
                   <c:v>5.0434615952563155E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5.001448083657245E-2</c:v>
+                  <c:v>5.0014480836572339E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>4.6484928838822326E-2</c:v>
@@ -2028,13 +2028,13 @@
                   <c:v>4.049533381557141E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3.4418892845651861E-2</c:v>
+                  <c:v>3.4418892845651972E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>2.904018514359763E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.4333977182246169E-2</c:v>
+                  <c:v>2.4333977182246114E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
                   <c:v>2.0673792478827779E-2</c:v>
@@ -2049,7 +2049,7 @@
                   <c:v>1.3615659272167902E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.1261997948185831E-2</c:v>
+                  <c:v>1.126199794818572E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>9.1062699711585982E-3</c:v>
@@ -3885,16 +3885,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3919,8 +3919,12 @@
       <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3928,23 +3932,22 @@
         <v>1.04506422</v>
       </c>
       <c r="C2">
-        <v>4.8174130799999997</v>
+        <v>8.4079719674640979E-2</v>
       </c>
       <c r="D2">
-        <v>-5.7954924300000004</v>
+        <v>-0.10115042467790698</v>
       </c>
       <c r="E2">
-        <v>-7.3353569399999996</v>
+        <v>-0.12802613041201613</v>
       </c>
       <c r="F2">
-        <v>5.3971079700000004</v>
+        <v>9.4197304162127349E-2</v>
       </c>
       <c r="G2">
-        <f>-C2-D2-E2</f>
-        <v>8.3134362900000003</v>
+        <v>0.14509683541528215</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H33" si="0">B2-$K$6*COS(RADIANS(C2+D2))-$K$7*COS(RADIANS(C2+D2+E2))-$K$10</f>
+        <f>B2-$K$6*COS(C2+D2)-$K$7*COS(C2+D2+E2)-$K$10</f>
         <v>7.116865845925302E-4</v>
       </c>
       <c r="J2" t="s">
@@ -3954,7 +3957,7 @@
         <v>0.1950308</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.699999999999996E-2</v>
       </c>
@@ -3962,23 +3965,22 @@
         <v>1.04418473</v>
       </c>
       <c r="C3">
-        <v>4.8074113699999996</v>
+        <v>8.3905156904311343E-2</v>
       </c>
       <c r="D3">
-        <v>-7.2844089199999997</v>
+        <v>-0.1271369197156442</v>
       </c>
       <c r="E3">
-        <v>-6.3340495299999997</v>
+        <v>-0.11055001928289934</v>
       </c>
       <c r="F3">
-        <v>5.6286378600000004</v>
+        <v>9.8238263059407638E-2</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G66" si="1">-C3-D3-E3</f>
-        <v>8.8110470799999998</v>
+        <v>0.15378178209423221</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H3:H66" si="0">B3-$K$6*COS(C3+D3)-$K$7*COS(C3+D3+E3)-$K$10</f>
         <v>9.1260743201959649E-4</v>
       </c>
       <c r="J3" t="s">
@@ -3988,7 +3990,7 @@
         <v>0.18455724409999999</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3.2999999999999974E-2</v>
       </c>
@@ -3996,20 +3998,19 @@
         <v>1.0426068799999999</v>
       </c>
       <c r="C4">
-        <v>4.7166309200000001</v>
+        <v>8.2320739155369263E-2</v>
       </c>
       <c r="D4">
-        <v>-8.7247815699999993</v>
+        <v>-0.15227616491382009</v>
       </c>
       <c r="E4">
-        <v>-5.3167808000000001</v>
+        <v>-9.2795330566818129E-2</v>
       </c>
       <c r="F4">
-        <v>5.8891238299999999</v>
+        <v>0.1027846008911588</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
-        <v>9.3249314499999993</v>
+        <v>0.16275075632526897</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
@@ -4023,7 +4024,7 @@
         <v>1.0449999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4.9999999999999989E-2</v>
       </c>
@@ -4031,27 +4032,26 @@
         <v>1.04088889</v>
       </c>
       <c r="C5">
-        <v>4.8409252599999997</v>
+        <v>8.4490084629962547E-2</v>
       </c>
       <c r="D5">
-        <v>-10.30761725</v>
+        <v>-0.17990185904786346</v>
       </c>
       <c r="E5">
-        <v>-4.4784145100000003</v>
+        <v>-7.8163078468588526E-2</v>
       </c>
       <c r="F5">
-        <v>6.24166928</v>
+        <v>0.10893767975658385</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
-        <v>9.9451065000000014</v>
+        <v>0.17357485288648947</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
         <v>1.1958020955685766E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6.7000000000000004E-2</v>
       </c>
@@ -4059,20 +4059,19 @@
         <v>1.0382929000000001</v>
       </c>
       <c r="C6">
-        <v>4.7052960600000002</v>
+        <v>8.2122908528116656E-2</v>
       </c>
       <c r="D6">
-        <v>-11.490597749999999</v>
+        <v>-0.20054876375975222</v>
       </c>
       <c r="E6">
-        <v>-3.8479056200000001</v>
+        <v>-6.7158622374993773E-2</v>
       </c>
       <c r="F6">
-        <v>6.6496922400000003</v>
+        <v>0.11605902383231699</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
-        <v>10.63320731</v>
+        <v>0.18558447760662936</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
@@ -4086,7 +4085,7 @@
         <v>0.53691676850156089</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>8.2999999999999963E-2</v>
       </c>
@@ -4094,20 +4093,19 @@
         <v>1.03586969</v>
       </c>
       <c r="C7">
-        <v>4.6381658300000002</v>
+        <v>8.0951264986995577E-2</v>
       </c>
       <c r="D7">
-        <v>-12.96257351</v>
+        <v>-0.22623958728129812</v>
       </c>
       <c r="E7">
-        <v>-2.9398076999999998</v>
+        <v>-5.1309323740481701E-2</v>
       </c>
       <c r="F7">
-        <v>6.9878691000000002</v>
+        <v>0.12196132349337288</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
-        <v>11.26421538</v>
+        <v>0.19659764603478422</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
@@ -4121,7 +4119,7 @@
         <v>0.50808323149843904</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>9.9999999999999978E-2</v>
       </c>
@@ -4129,20 +4127,19 @@
         <v>1.0328251100000001</v>
       </c>
       <c r="C8">
-        <v>4.4989094100000004</v>
+        <v>7.8520781953455507E-2</v>
       </c>
       <c r="D8">
-        <v>-14.381237779999999</v>
+        <v>-0.25099994977319995</v>
       </c>
       <c r="E8">
-        <v>-2.0765031199999999</v>
+        <v>-3.6241816371934917E-2</v>
       </c>
       <c r="F8">
-        <v>7.3261431999999997</v>
+        <v>0.12786532031259343</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
-        <v>11.95883149</v>
+        <v>0.20872098419167934</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
@@ -4153,10 +4150,10 @@
       </c>
       <c r="K8">
         <f>-H23/SIN(RADIANS(F23-G23))</f>
-        <v>0.18492841020407733</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>9.8258175170369704</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.11699999999999999</v>
       </c>
@@ -4164,27 +4161,26 @@
         <v>1.0292762</v>
       </c>
       <c r="C9">
-        <v>4.3558205299999999</v>
+        <v>7.6023409874464432E-2</v>
       </c>
       <c r="D9">
-        <v>-15.66585779</v>
+        <v>-0.27342079858470242</v>
       </c>
       <c r="E9">
-        <v>-1.4615201799999999</v>
+        <v>-2.5508339225340175E-2</v>
       </c>
       <c r="F9">
-        <v>7.7505187299999996</v>
+        <v>0.13527207057598939</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
-        <v>12.771557440000002</v>
+        <v>0.22290572793557817</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
         <v>2.5035843062888308E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.13300000000000001</v>
       </c>
@@ -4192,20 +4188,19 @@
         <v>1.0253583799999999</v>
       </c>
       <c r="C10">
-        <v>4.1862895900000003</v>
+        <v>7.3064536787463483E-2</v>
       </c>
       <c r="D10">
-        <v>-16.804714329999999</v>
+        <v>-0.29329759491557289</v>
       </c>
       <c r="E10">
-        <v>-1.13023352</v>
+        <v>-1.9726296240405179E-2</v>
       </c>
       <c r="F10">
-        <v>8.3186718899999992</v>
+        <v>0.14518821387359954</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
-        <v>13.748658259999999</v>
+        <v>0.23995935436851457</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
@@ -4218,7 +4213,7 @@
         <v>4.7697474025435449E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.15000000000000002</v>
       </c>
@@ -4226,27 +4221,26 @@
         <v>1.02137934</v>
       </c>
       <c r="C11">
-        <v>4.1029665399999997</v>
+        <v>7.1610275222159625E-2</v>
       </c>
       <c r="D11">
-        <v>-18.106946780000001</v>
+        <v>-0.31602583879438534</v>
       </c>
       <c r="E11">
-        <v>-0.73637821999999997</v>
+        <v>-1.2852224478975157E-2</v>
       </c>
       <c r="F11">
-        <v>8.7738972499999992</v>
+        <v>0.15313339524417602</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
-        <v>14.740358460000001</v>
+        <v>0.25726778805120093</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
         <v>4.2889845957959638E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.16699999999999993</v>
       </c>
@@ -4254,20 +4248,19 @@
         <v>1.0174538200000001</v>
       </c>
       <c r="C12">
-        <v>4.0254982000000004</v>
+        <v>7.0258197623105201E-2</v>
       </c>
       <c r="D12">
-        <v>-19.187784799999999</v>
+        <v>-0.33489002092412168</v>
       </c>
       <c r="E12">
-        <v>-0.77348927000000001</v>
+        <v>-1.3499934490347401E-2</v>
       </c>
       <c r="F12">
-        <v>9.4010041999999991</v>
+        <v>0.16407847628381547</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
-        <v>15.935775869999999</v>
+        <v>0.27813175779136384</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
@@ -4280,7 +4273,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.18299999999999994</v>
       </c>
@@ -4288,20 +4281,19 @@
         <v>1.0139772199999999</v>
       </c>
       <c r="C13">
-        <v>3.8765221099999998</v>
+        <v>6.7658074345857799E-2</v>
       </c>
       <c r="D13">
-        <v>-19.743247279999999</v>
+        <v>-0.34458467007141474</v>
       </c>
       <c r="E13">
-        <v>-1.63812655</v>
+        <v>-2.8590701861835512E-2</v>
       </c>
       <c r="F13">
-        <v>10.27956803</v>
+        <v>0.17941230780624723</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
-        <v>17.504851719999998</v>
+        <v>0.30551729758739249</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
@@ -4314,7 +4306,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.19999999999999996</v>
       </c>
@@ -4322,27 +4314,26 @@
         <v>1.01125686</v>
       </c>
       <c r="C14">
-        <v>3.8681001799999999</v>
+        <v>6.7511083937985314E-2</v>
       </c>
       <c r="D14">
-        <v>-20.676450809999999</v>
+        <v>-0.36087214426114844</v>
       </c>
       <c r="E14">
-        <v>-2.2575280000000002</v>
+        <v>-3.9401296555962549E-2</v>
       </c>
       <c r="F14">
-        <v>10.829402760000001</v>
+        <v>0.18900873418656128</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
-        <v>19.06587863</v>
+        <v>0.3327623568791257</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
         <v>1.2297223767784748E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.21699999999999997</v>
       </c>
@@ -4350,27 +4341,26 @@
         <v>1.0089246999999999</v>
       </c>
       <c r="C15">
-        <v>3.7733787099999998</v>
+        <v>6.5857882414156271E-2</v>
       </c>
       <c r="D15">
-        <v>-21.177009170000002</v>
+        <v>-0.36960853574153163</v>
       </c>
       <c r="E15">
-        <v>-3.5050767299999999</v>
+        <v>-6.1175129473536302E-2</v>
       </c>
       <c r="F15">
-        <v>11.54983425</v>
+        <v>0.20158263572210985</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
-        <v>20.908707190000001</v>
+        <v>0.36492578280091165</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
         <v>1.7191415794078901E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.23299999999999998</v>
       </c>
@@ -4378,20 +4368,19 @@
         <v>1.0073802300000001</v>
       </c>
       <c r="C16">
-        <v>3.7359598599999999</v>
+        <v>6.52048002793464E-2</v>
       </c>
       <c r="D16">
-        <v>-21.552394490000001</v>
+        <v>-0.37616024553918409</v>
       </c>
       <c r="E16">
-        <v>-5.0853297700000004</v>
+        <v>-8.8755748036185966E-2</v>
       </c>
       <c r="F16">
-        <v>12.036596660000001</v>
+        <v>0.21007824245155246</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
-        <v>22.901764400000001</v>
+        <v>0.39971119329602367</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
@@ -4406,20 +4395,19 @@
         <v>1.00611505</v>
       </c>
       <c r="C17">
-        <v>3.6110287900000002</v>
+        <v>6.3024341769806883E-2</v>
       </c>
       <c r="D17">
-        <v>-21.725710639999999</v>
+        <v>-0.37918518300356446</v>
       </c>
       <c r="E17">
-        <v>-6.87806066</v>
+        <v>-0.12004480466889424</v>
       </c>
       <c r="F17">
-        <v>12.349784939999999</v>
+        <v>0.21554440911621034</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
-        <v>24.992742509999999</v>
+        <v>0.43620564590265176</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
@@ -4434,20 +4422,19 @@
         <v>1.00553052</v>
       </c>
       <c r="C18">
-        <v>3.4673129899999999</v>
+        <v>6.0516027872669222E-2</v>
       </c>
       <c r="D18">
-        <v>-21.666035109999999</v>
+        <v>-0.37814364852219179</v>
       </c>
       <c r="E18">
-        <v>-9.0942442099999994</v>
+        <v>-0.15872450444493061</v>
       </c>
       <c r="F18">
-        <v>12.35009217</v>
+        <v>0.21554977129127126</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
-        <v>27.292966329999999</v>
+        <v>0.47635212509445313</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
@@ -4462,20 +4449,19 @@
         <v>1.00570519</v>
       </c>
       <c r="C19">
-        <v>3.54349063</v>
+        <v>6.1845578507068157E-2</v>
       </c>
       <c r="D19">
-        <v>-21.4672716</v>
+        <v>-0.37467457083987116</v>
       </c>
       <c r="E19">
-        <v>-11.97663313</v>
+        <v>-0.20903168142193404</v>
       </c>
       <c r="F19">
-        <v>12.06273612</v>
+        <v>0.21053446209324581</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
-        <v>29.900414099999999</v>
+        <v>0.52186067375473699</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
@@ -4490,24 +4476,23 @@
         <v>1.00698559</v>
       </c>
       <c r="C20">
-        <v>3.8205187500000002</v>
+        <v>6.6680631321678119E-2</v>
       </c>
       <c r="D20">
-        <v>-21.204207920000002</v>
+        <v>-0.37008324348145843</v>
       </c>
       <c r="E20">
-        <v>-15.43707124</v>
+        <v>-0.26942772000292381</v>
       </c>
       <c r="F20">
-        <v>11.27932942</v>
+        <v>0.19686143579606236</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
-        <v>32.820760409999998</v>
+        <v>0.57283033216270407</v>
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
-        <v>6.2844480971263939E-2</v>
+        <v>6.2844480971263994E-2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -4518,20 +4503,19 @@
         <v>1.0087757500000001</v>
       </c>
       <c r="C21">
-        <v>4.10151355</v>
+        <v>7.1584915762661072E-2</v>
       </c>
       <c r="D21">
-        <v>-20.33311836</v>
+        <v>-0.35487986257970972</v>
       </c>
       <c r="E21">
-        <v>-19.8812809</v>
+        <v>-0.34699381121886147</v>
       </c>
       <c r="F21">
-        <v>10.01895041</v>
+        <v>0.1748636722485358</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
-        <v>36.11288571</v>
+        <v>0.63028875803591011</v>
       </c>
       <c r="H21">
         <f t="shared" si="0"/>
@@ -4546,20 +4530,19 @@
         <v>1.01032207</v>
       </c>
       <c r="C22">
-        <v>4.2028951699999997</v>
+        <v>7.3354358832666805E-2</v>
       </c>
       <c r="D22">
-        <v>-18.321879169999999</v>
+        <v>-0.31977711666906583</v>
       </c>
       <c r="E22">
-        <v>-25.84635694</v>
+        <v>-0.45110402824868645</v>
       </c>
       <c r="F22">
-        <v>8.2662403900000001</v>
+        <v>0.14427311156684014</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
-        <v>39.965340939999997</v>
+        <v>0.69752678608508545</v>
       </c>
       <c r="H22">
         <f t="shared" si="0"/>
@@ -4574,20 +4557,19 @@
         <v>1.0122621300000001</v>
       </c>
       <c r="C23">
-        <v>4.29902447</v>
+        <v>7.5032131625304185E-2</v>
       </c>
       <c r="D23">
-        <v>-15.89824746</v>
+        <v>-0.27747676347382549</v>
       </c>
       <c r="E23">
-        <v>-32.149247889999998</v>
+        <v>-0.5611102277203398</v>
       </c>
       <c r="F23">
-        <v>5.4897559500000002</v>
+        <v>9.5814316458449206E-2</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
-        <v>43.748470879999999</v>
+        <v>0.76355485956886104</v>
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
@@ -4602,20 +4584,19 @@
         <v>1.0140218599999999</v>
       </c>
       <c r="C24">
-        <v>4.2234695899999997</v>
+        <v>7.3713450203354972E-2</v>
       </c>
       <c r="D24">
-        <v>-12.72118918</v>
+        <v>-0.22202663596007757</v>
       </c>
       <c r="E24">
-        <v>-38.889407429999999</v>
+        <v>-0.67874820380304612</v>
       </c>
       <c r="F24">
-        <v>1.8680845800000001</v>
+        <v>3.2604226626735414E-2</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
-        <v>47.387127019999994</v>
+        <v>0.82706138955976882</v>
       </c>
       <c r="H24">
         <f t="shared" si="0"/>
@@ -4630,20 +4611,19 @@
         <v>1.01579051</v>
       </c>
       <c r="C25">
-        <v>4.1593639099999997</v>
+        <v>7.2594595018125097E-2</v>
       </c>
       <c r="D25">
-        <v>-9.2937855099999993</v>
+        <v>-0.16220715712364037</v>
       </c>
       <c r="E25">
-        <v>-45.388824479999997</v>
+        <v>-0.79218443078580303</v>
       </c>
       <c r="F25">
-        <v>-2.03430219</v>
+        <v>-3.5505271196031266E-2</v>
       </c>
       <c r="G25">
-        <f t="shared" si="1"/>
-        <v>50.523246079999993</v>
+        <v>0.88179699289131819</v>
       </c>
       <c r="H25">
         <f t="shared" si="0"/>
@@ -4658,20 +4638,19 @@
         <v>1.01756723</v>
       </c>
       <c r="C26">
-        <v>4.1801128399999996</v>
+        <v>7.2956732162890919E-2</v>
       </c>
       <c r="D26">
-        <v>-5.9774851800000004</v>
+        <v>-0.1043267973801659</v>
       </c>
       <c r="E26">
-        <v>-51.33433694</v>
+        <v>-0.89595319893115077</v>
       </c>
       <c r="F26">
-        <v>-5.4194543299999998</v>
+        <v>-9.4587321719963299E-2</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
-        <v>53.131709280000003</v>
+        <v>0.92732326414842581</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
@@ -4686,20 +4665,19 @@
         <v>1.01996876</v>
       </c>
       <c r="C27">
-        <v>4.2644876900000002</v>
+        <v>7.4429351101267263E-2</v>
       </c>
       <c r="D27">
-        <v>-2.9672652400000001</v>
+        <v>-5.1788548217979749E-2</v>
       </c>
       <c r="E27">
-        <v>-56.323018320000003</v>
+        <v>-0.98302211434508524</v>
       </c>
       <c r="F27">
-        <v>-7.40786371</v>
+        <v>-0.12929161227850239</v>
       </c>
       <c r="G27">
-        <f t="shared" si="1"/>
-        <v>55.025795870000003</v>
+        <v>0.96038131146179773</v>
       </c>
       <c r="H27">
         <f t="shared" si="0"/>
@@ -4714,24 +4692,23 @@
         <v>1.0227400600000001</v>
       </c>
       <c r="C28">
-        <v>4.3678784100000003</v>
+        <v>7.6233859581274821E-2</v>
       </c>
       <c r="D28">
-        <v>-0.15939524999999999</v>
+        <v>-2.7819719245394912E-3</v>
       </c>
       <c r="E28">
-        <v>-60.501500399999998</v>
+        <v>-1.0559503843766662</v>
       </c>
       <c r="F28">
-        <v>-7.78985196</v>
+        <v>-0.13595856494493361</v>
       </c>
       <c r="G28">
-        <f t="shared" si="1"/>
-        <v>56.293017239999998</v>
+        <v>0.98249849671993095</v>
       </c>
       <c r="H28">
         <f t="shared" si="0"/>
-        <v>0.20054261109685689</v>
+        <v>0.20054261109685678</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -4742,24 +4719,23 @@
         <v>1.02585818</v>
       </c>
       <c r="C29">
-        <v>4.4865816599999997</v>
+        <v>7.8305622126592769E-2</v>
       </c>
       <c r="D29">
-        <v>2.4413810300000001</v>
+        <v>4.2610137269230457E-2</v>
       </c>
       <c r="E29">
-        <v>-63.865174000000003</v>
+        <v>-1.1146575636590772</v>
       </c>
       <c r="F29">
-        <v>-6.8791489099999996</v>
+        <v>-0.12006379821447907</v>
       </c>
       <c r="G29">
-        <f t="shared" si="1"/>
-        <v>56.937211310000002</v>
+        <v>0.99374180426325387</v>
       </c>
       <c r="H29">
         <f t="shared" si="0"/>
-        <v>0.21090315205236621</v>
+        <v>0.21090315205236626</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -4770,20 +4746,19 @@
         <v>1.02920966</v>
       </c>
       <c r="C30">
-        <v>4.6724272300000003</v>
+        <v>8.1549239223338371E-2</v>
       </c>
       <c r="D30">
-        <v>4.7689030700000004</v>
+        <v>8.3233060279965632E-2</v>
       </c>
       <c r="E30">
-        <v>-66.334021070000006</v>
+        <v>-1.157747073758792</v>
       </c>
       <c r="F30">
-        <v>-5.3871736099999996</v>
+        <v>-9.4023916871048913E-2</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
-        <v>56.892690770000002</v>
+        <v>0.9929647742554879</v>
       </c>
       <c r="H30">
         <f t="shared" si="0"/>
@@ -4798,24 +4773,23 @@
         <v>1.0324374199999999</v>
       </c>
       <c r="C31">
-        <v>4.6868031400000003</v>
+        <v>8.1800146185808748E-2</v>
       </c>
       <c r="D31">
-        <v>7.2178498400000004</v>
+        <v>0.12597524462254592</v>
       </c>
       <c r="E31">
-        <v>-68.022329049999996</v>
+        <v>-1.1872136067974866</v>
       </c>
       <c r="F31">
-        <v>-3.85984046</v>
+        <v>-6.7366924628692482E-2</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
-        <v>56.117676069999995</v>
+        <v>0.97943821598913172</v>
       </c>
       <c r="H31">
         <f t="shared" si="0"/>
-        <v>0.21904796091100515</v>
+        <v>0.2190479609110052</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -4826,24 +4800,23 @@
         <v>1.03561101</v>
       </c>
       <c r="C32">
-        <v>4.8550686799999996</v>
+        <v>8.4736933876454951E-2</v>
       </c>
       <c r="D32">
-        <v>9.2852722700000001</v>
+        <v>0.1620585730556279</v>
       </c>
       <c r="E32">
-        <v>-68.871945479999994</v>
+        <v>-1.2020422108800262</v>
       </c>
       <c r="F32">
-        <v>-2.5251686900000001</v>
+        <v>-4.4072507808772012E-2</v>
       </c>
       <c r="G32">
-        <f t="shared" si="1"/>
-        <v>54.731604529999998</v>
+        <v>0.95524670394794353</v>
       </c>
       <c r="H32">
         <f t="shared" si="0"/>
-        <v>0.21682194449721637</v>
+        <v>0.21682194449721626</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -4854,24 +4827,23 @@
         <v>1.0382935600000001</v>
       </c>
       <c r="C33">
-        <v>4.8889317300000004</v>
+        <v>8.5327955593722443E-2</v>
       </c>
       <c r="D33">
-        <v>11.38041372</v>
+        <v>0.19862568965313607</v>
       </c>
       <c r="E33">
-        <v>-68.92268018</v>
+        <v>-1.2029276984400379</v>
       </c>
       <c r="F33">
-        <v>-1.45200182</v>
+        <v>-2.5342212503950051E-2</v>
       </c>
       <c r="G33">
-        <f t="shared" si="1"/>
-        <v>52.653334729999997</v>
+        <v>0.91897405319317937</v>
       </c>
       <c r="H33">
         <f t="shared" si="0"/>
-        <v>0.20988608432065931</v>
+        <v>0.20988608432065936</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -4882,24 +4854,23 @@
         <v>1.04078538</v>
       </c>
       <c r="C34">
-        <v>4.9215114199999999</v>
+        <v>8.5896578453501501E-2</v>
       </c>
       <c r="D34">
-        <v>13.221542769999999</v>
+        <v>0.23075945352975136</v>
       </c>
       <c r="E34">
-        <v>-68.101411760000005</v>
+        <v>-1.1885938604683866</v>
       </c>
       <c r="F34">
-        <v>-0.64256811000000003</v>
+        <v>-1.1214929187817101E-2</v>
       </c>
       <c r="G34">
-        <f t="shared" si="1"/>
-        <v>49.958357570000004</v>
+        <v>0.87193782848513357</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34:H65" si="2">B34-$K$6*COS(RADIANS(C34+D34))-$K$7*COS(RADIANS(C34+D34+E34))-$K$10</f>
-        <v>0.19892088731401653</v>
+        <f t="shared" si="0"/>
+        <v>0.19892088731401658</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -4910,23 +4881,22 @@
         <v>1.04210245</v>
       </c>
       <c r="C35">
-        <v>4.7493412700000004</v>
+        <v>8.2891642462348994E-2</v>
       </c>
       <c r="D35">
-        <v>15.11003644</v>
+        <v>0.26371988597432261</v>
       </c>
       <c r="E35">
-        <v>-66.59332345</v>
+        <v>-1.1622727540480493</v>
       </c>
       <c r="F35">
-        <v>-1.4047489999999999E-2</v>
+        <v>-2.4517495214097822E-4</v>
       </c>
       <c r="G35">
-        <f t="shared" si="1"/>
-        <v>46.733945739999996</v>
+        <v>0.81566122561137777</v>
       </c>
       <c r="H35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.18411312598422808</v>
       </c>
     </row>
@@ -4938,23 +4908,22 @@
         <v>1.0429828000000001</v>
       </c>
       <c r="C36">
-        <v>4.5879994599999998</v>
+        <v>8.0075696656721873E-2</v>
       </c>
       <c r="D36">
-        <v>16.860523019999999</v>
+        <v>0.29427164030729769</v>
       </c>
       <c r="E36">
-        <v>-64.429180389999999</v>
+        <v>-1.1245013321668642</v>
       </c>
       <c r="F36">
-        <v>0.50279784000000005</v>
+        <v>8.7754777799156462E-3</v>
       </c>
       <c r="G36">
-        <f t="shared" si="1"/>
-        <v>42.980657910000005</v>
+        <v>0.75015399520284476</v>
       </c>
       <c r="H36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.1667741547718396</v>
       </c>
     </row>
@@ -4966,24 +4935,23 @@
         <v>1.0441639599999999</v>
       </c>
       <c r="C37">
-        <v>4.79493189</v>
+        <v>8.3687348889374569E-2</v>
       </c>
       <c r="D37">
-        <v>17.76543083</v>
+        <v>0.31006526101880899</v>
       </c>
       <c r="E37">
-        <v>-61.395405169999997</v>
+        <v>-1.0715519658124488</v>
       </c>
       <c r="F37">
-        <v>1.0623400999999999</v>
+        <v>1.8541332520965809E-2</v>
       </c>
       <c r="G37">
-        <f t="shared" si="1"/>
-        <v>38.835042449999996</v>
+        <v>0.67779935590426521</v>
       </c>
       <c r="H37">
-        <f t="shared" si="2"/>
-        <v>0.14779077984641925</v>
+        <f t="shared" si="0"/>
+        <v>0.1477907798464192</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -4994,24 +4962,23 @@
         <v>1.0445616799999999</v>
       </c>
       <c r="C38">
-        <v>4.8793311099999999</v>
+        <v>8.5160393164489617E-2</v>
       </c>
       <c r="D38">
-        <v>18.743883310000001</v>
+        <v>0.32714247836911298</v>
       </c>
       <c r="E38">
-        <v>-57.772776970000002</v>
+        <v>-1.0083251761468535</v>
       </c>
       <c r="F38">
-        <v>1.4322887799999999</v>
+        <v>2.4998155050372704E-2</v>
       </c>
       <c r="G38">
-        <f t="shared" si="1"/>
-        <v>34.149562549999999</v>
+        <v>0.59602230461325068</v>
       </c>
       <c r="H38">
-        <f t="shared" si="2"/>
-        <v>0.12739154148061121</v>
+        <f t="shared" si="0"/>
+        <v>0.12739154148061127</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -5022,24 +4989,23 @@
         <v>1.04449532</v>
       </c>
       <c r="C39">
-        <v>4.9357090399999999</v>
+        <v>8.6144373668448501E-2</v>
       </c>
       <c r="D39">
-        <v>19.4297483</v>
+        <v>0.33911308066877094</v>
       </c>
       <c r="E39">
-        <v>-53.511960870000003</v>
+        <v>-0.93395990637986925</v>
       </c>
       <c r="F39">
-        <v>1.6734766000000001</v>
+        <v>2.9207676625080139E-2</v>
       </c>
       <c r="G39">
-        <f t="shared" si="1"/>
-        <v>29.146503530000004</v>
+        <v>0.50870245204264997</v>
       </c>
       <c r="H39">
-        <f t="shared" si="2"/>
-        <v>0.10688229884476697</v>
+        <f t="shared" si="0"/>
+        <v>0.10688229884476691</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -5050,23 +5016,22 @@
         <v>1.04396621</v>
       </c>
       <c r="C40">
-        <v>4.9549174699999998</v>
+        <v>8.6479624016087359E-2</v>
       </c>
       <c r="D40">
-        <v>19.9490433</v>
+        <v>0.34817648820791491</v>
       </c>
       <c r="E40">
-        <v>-48.753094689999998</v>
+        <v>-0.85090202287706418</v>
       </c>
       <c r="F40">
-        <v>1.62652413</v>
+        <v>2.8388201431636277E-2</v>
       </c>
       <c r="G40">
-        <f t="shared" si="1"/>
-        <v>23.84913392</v>
+        <v>0.41624591065306188</v>
       </c>
       <c r="H40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>8.7505283312476922E-2</v>
       </c>
     </row>
@@ -5078,23 +5043,22 @@
         <v>1.0432965300000001</v>
       </c>
       <c r="C41">
-        <v>5.0949008200000003</v>
+        <v>8.8922794371558964E-2</v>
       </c>
       <c r="D41">
-        <v>20.0939376</v>
+        <v>0.35070537081028735</v>
       </c>
       <c r="E41">
-        <v>-43.478738640000003</v>
+        <v>-0.75884714388208163</v>
       </c>
       <c r="F41">
-        <v>1.2680068</v>
+        <v>2.2130893597677233E-2</v>
       </c>
       <c r="G41">
-        <f t="shared" si="1"/>
-        <v>18.289900220000003</v>
+        <v>0.31921897870023525</v>
       </c>
       <c r="H41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7.025016139349255E-2</v>
       </c>
     </row>
@@ -5106,24 +5070,23 @@
         <v>1.0415996000000001</v>
       </c>
       <c r="C42">
-        <v>4.9693523600000002</v>
+        <v>8.6731560373750571E-2</v>
       </c>
       <c r="D42">
-        <v>20.36268527</v>
+        <v>0.3553959025088505</v>
       </c>
       <c r="E42">
-        <v>-37.970675720000003</v>
+        <v>-0.66271331052106852</v>
       </c>
       <c r="F42">
-        <v>0.73223274000000005</v>
+        <v>1.2779872203899584E-2</v>
       </c>
       <c r="G42">
-        <f t="shared" si="1"/>
-        <v>12.638638090000001</v>
+        <v>0.22058584763846742</v>
       </c>
       <c r="H42">
-        <f t="shared" si="2"/>
-        <v>5.5769063846833278E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.5769063846833167E-2</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -5134,23 +5097,22 @@
         <v>1.03967831</v>
       </c>
       <c r="C43">
-        <v>4.8880476599999998</v>
+        <v>8.5312525661404334E-2</v>
       </c>
       <c r="D43">
-        <v>20.30613486</v>
+        <v>0.35440891166099781</v>
       </c>
       <c r="E43">
-        <v>-32.062752109999998</v>
+        <v>-0.5596005915702591</v>
       </c>
       <c r="F43">
-        <v>-3.3072379999999998E-2</v>
+        <v>-5.7722192247072225E-4</v>
       </c>
       <c r="G43">
-        <f t="shared" si="1"/>
-        <v>6.8685695899999999</v>
+        <v>0.11987915424785699</v>
       </c>
       <c r="H43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>4.4631769934232235E-2</v>
       </c>
     </row>
@@ -5162,23 +5124,22 @@
         <v>1.03725673</v>
       </c>
       <c r="C44">
-        <v>4.7522101699999997</v>
+        <v>8.2941714213259451E-2</v>
       </c>
       <c r="D44">
-        <v>20.28468956</v>
+        <v>0.35403462056691987</v>
       </c>
       <c r="E44">
-        <v>-26.32450892</v>
+        <v>-0.4594493546246165</v>
       </c>
       <c r="F44">
-        <v>-0.71563701000000002</v>
+        <v>-1.2490222073627585E-2</v>
       </c>
       <c r="G44">
-        <f t="shared" si="1"/>
-        <v>1.2876091899999977</v>
+        <v>2.2473019844437205E-2</v>
       </c>
       <c r="H44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3.8066434157436269E-2</v>
       </c>
     </row>
@@ -5190,23 +5151,22 @@
         <v>1.0344577399999999</v>
       </c>
       <c r="C45">
-        <v>4.5504512200000002</v>
+        <v>7.9420356240392842E-2</v>
       </c>
       <c r="D45">
-        <v>20.188299910000001</v>
+        <v>0.35235230380957494</v>
       </c>
       <c r="E45">
-        <v>-20.504041820000001</v>
+        <v>-0.35786303972561051</v>
       </c>
       <c r="F45">
-        <v>-1.3262094499999999</v>
+        <v>-2.3146721473563107E-2</v>
       </c>
       <c r="G45">
-        <f t="shared" si="1"/>
-        <v>-4.2347093099999995</v>
+        <v>-7.3909620324357217E-2</v>
       </c>
       <c r="H45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3.5350444430718553E-2</v>
       </c>
     </row>
@@ -5218,23 +5178,22 @@
         <v>1.03138866</v>
       </c>
       <c r="C46">
-        <v>4.40613016</v>
+        <v>7.6901478563424552E-2</v>
       </c>
       <c r="D46">
-        <v>20.03529644</v>
+        <v>0.34968188949109852</v>
       </c>
       <c r="E46">
-        <v>-15.097056540000001</v>
+        <v>-0.26349334398274299</v>
       </c>
       <c r="F46">
-        <v>-1.6293674300000001</v>
+        <v>-2.8437826378258233E-2</v>
       </c>
       <c r="G46">
-        <f t="shared" si="1"/>
-        <v>-9.3443700599999993</v>
+        <v>-0.16309002407178005</v>
       </c>
       <c r="H46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3.6476976040728082E-2</v>
       </c>
     </row>
@@ -5246,23 +5205,22 @@
         <v>1.0284736999999999</v>
       </c>
       <c r="C47">
-        <v>4.4635900299999998</v>
+        <v>7.7904342482692471E-2</v>
       </c>
       <c r="D47">
-        <v>19.50350392</v>
+        <v>0.34040035907962074</v>
       </c>
       <c r="E47">
-        <v>-9.9113464699999998</v>
+        <v>-0.17298562920741736</v>
       </c>
       <c r="F47">
-        <v>-1.7383312399999999</v>
+        <v>-3.0339603628275751E-2</v>
       </c>
       <c r="G47">
-        <f t="shared" si="1"/>
-        <v>-14.055747479999999</v>
+        <v>-0.24531907235489581</v>
       </c>
       <c r="H47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>4.020957671277603E-2</v>
       </c>
     </row>
@@ -5274,24 +5232,23 @@
         <v>1.02518753</v>
       </c>
       <c r="C48">
-        <v>4.4274746199999999</v>
+        <v>7.727400966748478E-2</v>
       </c>
       <c r="D48">
-        <v>19.137302420000001</v>
+        <v>0.33400893717887875</v>
       </c>
       <c r="E48">
-        <v>-5.6884190600000002</v>
+        <v>-9.928164183020087E-2</v>
       </c>
       <c r="F48">
-        <v>-1.5202655599999999</v>
+        <v>-2.6533639526675402E-2</v>
       </c>
       <c r="G48">
-        <f t="shared" si="1"/>
-        <v>-17.876357980000002</v>
+        <v>-0.31200130501616263</v>
       </c>
       <c r="H48">
-        <f t="shared" si="2"/>
-        <v>4.4721659343532505E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.4721659343532338E-2</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -5302,23 +5259,22 @@
         <v>1.02230076</v>
       </c>
       <c r="C49">
-        <v>4.5446272700000003</v>
+        <v>7.9318709137421325E-2</v>
       </c>
       <c r="D49">
-        <v>18.686110729999999</v>
+        <v>0.32613415663074113</v>
       </c>
       <c r="E49">
-        <v>-2.5864982900000002</v>
+        <v>-4.5142911257703124E-2</v>
       </c>
       <c r="F49">
-        <v>-1.1193859799999999</v>
+        <v>-1.9536970951663395E-2</v>
       </c>
       <c r="G49">
-        <f t="shared" si="1"/>
-        <v>-20.644239709999997</v>
+        <v>-0.36030995451045933</v>
       </c>
       <c r="H49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>4.8687397744538286E-2</v>
       </c>
     </row>
@@ -5330,23 +5286,22 @@
         <v>1.0192673699999999</v>
       </c>
       <c r="C50">
-        <v>4.4372021500000001</v>
+        <v>7.7443787094071306E-2</v>
       </c>
       <c r="D50">
-        <v>18.608190700000002</v>
+        <v>0.3247741955539884</v>
       </c>
       <c r="E50">
-        <v>-0.71905746999999998</v>
+        <v>-1.2549920362560351E-2</v>
       </c>
       <c r="F50">
-        <v>-0.75749562000000004</v>
+        <v>-1.322079263843581E-2</v>
       </c>
       <c r="G50">
-        <f t="shared" si="1"/>
-        <v>-22.326335380000003</v>
+        <v>-0.38966806228549938</v>
       </c>
       <c r="H50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5.0434615952563155E-2</v>
       </c>
     </row>
@@ -5358,24 +5313,23 @@
         <v>1.0170378099999999</v>
       </c>
       <c r="C51">
-        <v>4.5679405099999997</v>
+        <v>7.9725601934728954E-2</v>
       </c>
       <c r="D51">
-        <v>18.666677870000001</v>
+        <v>0.32579498924066203</v>
       </c>
       <c r="E51">
-        <v>-0.58029452000000004</v>
+        <v>-1.0128050005280087E-2</v>
       </c>
       <c r="F51">
-        <v>-0.42661675999999998</v>
+        <v>-7.4458671061904437E-3</v>
       </c>
       <c r="G51">
-        <f t="shared" si="1"/>
-        <v>-22.654323860000002</v>
+        <v>-0.39539254117011097</v>
       </c>
       <c r="H51">
-        <f t="shared" si="2"/>
-        <v>5.001448083657245E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.0014480836572339E-2</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -5386,23 +5340,22 @@
         <v>1.01517726</v>
       </c>
       <c r="C52">
-        <v>4.6466512</v>
+        <v>8.1099362631745539E-2</v>
       </c>
       <c r="D52">
-        <v>18.829657879999999</v>
+        <v>0.3286395270300953</v>
       </c>
       <c r="E52">
-        <v>-1.5857218900000001</v>
+        <v>-2.7676068001447347E-2</v>
       </c>
       <c r="F52">
-        <v>-0.42494636000000002</v>
+        <v>-7.416713126365132E-3</v>
       </c>
       <c r="G52">
-        <f t="shared" si="1"/>
-        <v>-21.890587190000002</v>
+        <v>-0.38206282166039351</v>
       </c>
       <c r="H52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>4.6484928838822326E-2</v>
       </c>
     </row>
@@ -5414,23 +5367,22 @@
         <v>1.01374181</v>
       </c>
       <c r="C53">
-        <v>4.58086488</v>
+        <v>7.9951174744974943E-2</v>
       </c>
       <c r="D53">
-        <v>19.100652180000001</v>
+        <v>0.33336926981923259</v>
       </c>
       <c r="E53">
-        <v>-3.4619205499999999</v>
+        <v>-6.042191203995298E-2</v>
       </c>
       <c r="F53">
-        <v>-0.79356762000000003</v>
+        <v>-1.3850367806215205E-2</v>
       </c>
       <c r="G53">
-        <f t="shared" si="1"/>
-        <v>-20.219596510000002</v>
+        <v>-0.35289853252425457</v>
       </c>
       <c r="H53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>4.049533381557141E-2</v>
       </c>
     </row>
@@ -5442,24 +5394,23 @@
         <v>1.0123922400000001</v>
       </c>
       <c r="C54">
-        <v>4.4345428900000003</v>
+        <v>7.7397374251404735E-2</v>
       </c>
       <c r="D54">
-        <v>19.66008837</v>
+        <v>0.34313327328954518</v>
       </c>
       <c r="E54">
-        <v>-6.0404142199999997</v>
+        <v>-0.10542511632328511</v>
       </c>
       <c r="F54">
-        <v>-1.55981579</v>
+        <v>-2.7223921260096439E-2</v>
       </c>
       <c r="G54">
-        <f t="shared" si="1"/>
-        <v>-18.054217040000001</v>
+        <v>-0.31510553121766477</v>
       </c>
       <c r="H54">
-        <f t="shared" si="2"/>
-        <v>3.4418892845651861E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.4418892845651972E-2</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
@@ -5470,23 +5421,22 @@
         <v>1.01141057</v>
       </c>
       <c r="C55">
-        <v>4.2150832100000004</v>
+        <v>7.3567080260031573E-2</v>
       </c>
       <c r="D55">
-        <v>20.229378229999998</v>
+        <v>0.35306925574476272</v>
       </c>
       <c r="E55">
-        <v>-8.6133244599999994</v>
+        <v>-0.15033087136956261</v>
       </c>
       <c r="F55">
-        <v>-2.6721031599999998</v>
+        <v>-4.6636998094944843E-2</v>
       </c>
       <c r="G55">
-        <f t="shared" si="1"/>
-        <v>-15.831136979999998</v>
+        <v>-0.27630546463523165</v>
       </c>
       <c r="H55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2.904018514359763E-2</v>
       </c>
     </row>
@@ -5498,24 +5448,23 @@
         <v>1.01119859</v>
       </c>
       <c r="C56">
-        <v>4.1051098499999998</v>
+        <v>7.1647683038550541E-2</v>
       </c>
       <c r="D56">
-        <v>20.573107650000001</v>
+        <v>0.35906846585973318</v>
       </c>
       <c r="E56">
-        <v>-11.261302969999999</v>
+        <v>-0.19654681489111622</v>
       </c>
       <c r="F56">
-        <v>-3.51984582</v>
+        <v>-6.143289872155968E-2</v>
       </c>
       <c r="G56">
-        <f t="shared" si="1"/>
-        <v>-13.416914530000003</v>
+        <v>-0.23416933400716755</v>
       </c>
       <c r="H56">
-        <f t="shared" si="2"/>
-        <v>2.4333977182246169E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.4333977182246114E-2</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
@@ -5526,23 +5475,22 @@
         <v>1.01182485</v>
       </c>
       <c r="C57">
-        <v>4.2262142100000002</v>
+        <v>7.3761352859071067E-2</v>
       </c>
       <c r="D57">
-        <v>20.502663099999999</v>
+        <v>0.35783897652214741</v>
       </c>
       <c r="E57">
-        <v>-13.70105461</v>
+        <v>-0.23912851394004758</v>
       </c>
       <c r="F57">
-        <v>-4.0360431400000003</v>
+        <v>-7.0442241545530457E-2</v>
       </c>
       <c r="G57">
-        <f t="shared" si="1"/>
-        <v>-11.027822700000002</v>
+        <v>-0.1924718154411709</v>
       </c>
       <c r="H57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2.0673792478827779E-2</v>
       </c>
     </row>
@@ -5554,23 +5502,22 @@
         <v>1.0129916800000001</v>
       </c>
       <c r="C58">
-        <v>4.4287009900000003</v>
+        <v>7.7295413861832474E-2</v>
       </c>
       <c r="D58">
-        <v>20.175189159999999</v>
+        <v>0.35212347805466898</v>
       </c>
       <c r="E58">
-        <v>-15.89926923</v>
+        <v>-0.27749459672452359</v>
       </c>
       <c r="F58">
-        <v>-4.1311961699999999</v>
+        <v>-7.2102975212279388E-2</v>
       </c>
       <c r="G58">
-        <f t="shared" si="1"/>
-        <v>-8.7046209199999982</v>
+        <v>-0.15192429519197789</v>
       </c>
       <c r="H58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1.782202706937297E-2</v>
       </c>
     </row>
@@ -5582,23 +5529,22 @@
         <v>1.0149204599999999</v>
       </c>
       <c r="C59">
-        <v>4.8750458999999999</v>
+        <v>8.5085602140850231E-2</v>
       </c>
       <c r="D59">
-        <v>19.344886540000001</v>
+        <v>0.33763196354773378</v>
       </c>
       <c r="E59">
-        <v>-17.701204050000001</v>
+        <v>-0.30894429223985498</v>
       </c>
       <c r="F59">
-        <v>-3.8614800100000002</v>
+        <v>-6.7395540174443561E-2</v>
       </c>
       <c r="G59">
-        <f t="shared" si="1"/>
-        <v>-6.5187283899999997</v>
+        <v>-0.11377327344872898</v>
       </c>
       <c r="H59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1.5696353336845714E-2</v>
       </c>
     </row>
@@ -5610,23 +5556,22 @@
         <v>1.0167712499999999</v>
       </c>
       <c r="C60">
-        <v>5.1627252199999996</v>
+        <v>9.0106553464748607E-2</v>
       </c>
       <c r="D60">
-        <v>18.463576889999999</v>
+        <v>0.3222502084256349</v>
       </c>
       <c r="E60">
-        <v>-19.065023740000001</v>
+        <v>-0.33274743623388336</v>
       </c>
       <c r="F60">
-        <v>-3.3180530300000002</v>
+        <v>-5.7910950129274184E-2</v>
       </c>
       <c r="G60">
-        <f t="shared" si="1"/>
-        <v>-4.5612783699999966</v>
+        <v>-7.9609325656500085E-2</v>
       </c>
       <c r="H60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1.3615659272167902E-2</v>
       </c>
     </row>
@@ -5638,24 +5583,23 @@
         <v>1.01854651</v>
       </c>
       <c r="C61">
-        <v>5.3362687299999996</v>
+        <v>9.3135459109716295E-2</v>
       </c>
       <c r="D61">
-        <v>17.433584490000001</v>
+        <v>0.30427344977511644</v>
       </c>
       <c r="E61">
-        <v>-19.890018449999999</v>
+        <v>-0.34714631023491915</v>
       </c>
       <c r="F61">
-        <v>-2.5877221000000001</v>
+        <v>-4.516427077162196E-2</v>
       </c>
       <c r="G61">
-        <f t="shared" si="1"/>
-        <v>-2.8798347700000022</v>
+        <v>-5.0262598649913663E-2</v>
       </c>
       <c r="H61">
-        <f t="shared" si="2"/>
-        <v>1.1261997948185831E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.126199794818572E-2</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
@@ -5666,23 +5610,22 @@
         <v>1.02025268</v>
       </c>
       <c r="C62">
-        <v>5.4067614199999996</v>
+        <v>9.4365788648803989E-2</v>
       </c>
       <c r="D62">
-        <v>16.417915170000001</v>
+        <v>0.28654667602962458</v>
       </c>
       <c r="E62">
-        <v>-20.47837938</v>
+        <v>-0.35741514565351501</v>
       </c>
       <c r="F62">
-        <v>-1.6452306000000001</v>
+        <v>-2.8714690924561824E-2</v>
       </c>
       <c r="G62">
-        <f t="shared" si="1"/>
-        <v>-1.3462972099999995</v>
+        <v>-2.3497319024913518E-2</v>
       </c>
       <c r="H62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>9.1062699711585982E-3</v>
       </c>
     </row>
@@ -5694,23 +5637,22 @@
         <v>1.0227134200000001</v>
       </c>
       <c r="C63">
-        <v>5.6317307200000002</v>
+        <v>9.829224364971087E-2</v>
       </c>
       <c r="D63">
-        <v>14.867617259999999</v>
+        <v>0.25948887311333785</v>
       </c>
       <c r="E63">
-        <v>-20.324421839999999</v>
+        <v>-0.35472807967224412</v>
       </c>
       <c r="F63">
-        <v>-0.77333432000000002</v>
+        <v>-1.3497230102671435E-2</v>
       </c>
       <c r="G63">
-        <f t="shared" si="1"/>
-        <v>-0.17492614000000017</v>
+        <v>-3.0530370908045568E-3</v>
       </c>
       <c r="H63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>6.9456642771068555E-3</v>
       </c>
     </row>
@@ -5722,23 +5664,22 @@
         <v>1.0249600800000001</v>
       </c>
       <c r="C64">
-        <v>5.8024070600000002</v>
+        <v>0.10127110773796417</v>
       </c>
       <c r="D64">
-        <v>13.31228378</v>
+        <v>0.23234318292083647</v>
       </c>
       <c r="E64">
-        <v>-19.887226340000002</v>
+        <v>-0.34709757872234126</v>
       </c>
       <c r="F64">
-        <v>2.2360339999999999E-2</v>
+        <v>3.9026155486538881E-4</v>
       </c>
       <c r="G64">
-        <f t="shared" si="1"/>
-        <v>0.77253550000000004</v>
+        <v>1.3483288063540655E-2</v>
       </c>
       <c r="H64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>4.8394325101331903E-3</v>
       </c>
     </row>
@@ -5750,23 +5691,22 @@
         <v>1.0275626</v>
       </c>
       <c r="C65">
-        <v>5.9617183100000002</v>
+        <v>0.10405161358593198</v>
       </c>
       <c r="D65">
-        <v>11.72751959</v>
+        <v>0.20468382993763545</v>
       </c>
       <c r="E65">
-        <v>-19.358788369999999</v>
+        <v>-0.33787459625328625</v>
       </c>
       <c r="F65">
-        <v>0.80110055999999996</v>
+        <v>1.3981842411570385E-2</v>
       </c>
       <c r="G65">
-        <f t="shared" si="1"/>
-        <v>1.6695504699999972</v>
+        <v>2.9139152729718763E-2</v>
       </c>
       <c r="H65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3.39473300210269E-3</v>
       </c>
     </row>
@@ -5778,23 +5718,22 @@
         <v>1.0308441699999999</v>
       </c>
       <c r="C66">
-        <v>6.00848008</v>
+        <v>0.10486776043649229</v>
       </c>
       <c r="D66">
-        <v>10.089960039999999</v>
+        <v>0.17610302409265874</v>
       </c>
       <c r="E66">
-        <v>-18.617247389999999</v>
+        <v>-0.3249322646138208</v>
       </c>
       <c r="F66">
-        <v>1.51054746</v>
+        <v>2.6364026684637346E-2</v>
       </c>
       <c r="G66">
-        <f t="shared" si="1"/>
-        <v>2.5188072699999999</v>
+        <v>4.3961480084669789E-2</v>
       </c>
       <c r="H66">
-        <f t="shared" ref="H66:H74" si="3">B66-$K$6*COS(RADIANS(C66+D66))-$K$7*COS(RADIANS(C66+D66+E66))-$K$10</f>
+        <f t="shared" si="0"/>
         <v>2.6195836683922114E-3</v>
       </c>
     </row>
@@ -5806,23 +5745,22 @@
         <v>1.0341993300000001</v>
       </c>
       <c r="C67">
-        <v>6.2193765699999997</v>
+        <v>0.10854859856789158</v>
       </c>
       <c r="D67">
-        <v>8.1690495199999997</v>
+        <v>0.14257681088246238</v>
       </c>
       <c r="E67">
-        <v>-17.504483570000001</v>
+        <v>-0.30551087215775136</v>
       </c>
       <c r="F67">
-        <v>1.9925147599999999</v>
+        <v>3.4775942956584607E-2</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G74" si="4">-C67-D67-E67</f>
-        <v>3.116057480000002</v>
+        <v>5.4385462707397393E-2</v>
       </c>
       <c r="H67">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="H67:H74" si="1">B67-$K$6*COS(C67+D67)-$K$7*COS(C67+D67+E67)-$K$10</f>
         <v>2.0220618820427916E-3</v>
       </c>
     </row>
@@ -5834,23 +5772,22 @@
         <v>1.0368907000000001</v>
       </c>
       <c r="C68">
-        <v>6.1610436399999999</v>
+        <v>0.10753049687705622</v>
       </c>
       <c r="D68">
-        <v>6.6795832199999996</v>
+        <v>0.11658071984996475</v>
       </c>
       <c r="E68">
-        <v>-16.650372090000001</v>
+        <v>-0.29060381465266966</v>
       </c>
       <c r="F68">
-        <v>2.5513556799999999</v>
+        <v>4.4529557005458839E-2</v>
       </c>
       <c r="G68">
-        <f t="shared" si="4"/>
-        <v>3.8097452300000008</v>
+        <v>6.6492597925648669E-2</v>
       </c>
       <c r="H68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.6709306523434719E-3</v>
       </c>
     </row>
@@ -5862,23 +5799,22 @@
         <v>1.03952972</v>
       </c>
       <c r="C69">
-        <v>6.1908538799999997</v>
+        <v>0.10805078371586592</v>
       </c>
       <c r="D69">
-        <v>4.9621785999999997</v>
+        <v>8.6606354642002684E-2</v>
       </c>
       <c r="E69">
-        <v>-15.48992116</v>
+        <v>-0.27035012511633938</v>
       </c>
       <c r="F69">
-        <v>2.9746337899999999</v>
+        <v>5.1917153676577579E-2</v>
       </c>
       <c r="G69">
-        <f t="shared" si="4"/>
-        <v>4.3368886799999995</v>
+        <v>7.5692986758470748E-2</v>
       </c>
       <c r="H69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.3549758566331338E-3</v>
       </c>
     </row>
@@ -5890,23 +5826,22 @@
         <v>1.04185321</v>
       </c>
       <c r="C70">
-        <v>6.22635557</v>
+        <v>0.10867040509638827</v>
       </c>
       <c r="D70">
-        <v>3.1621432</v>
+        <v>5.5189810259549554E-2</v>
       </c>
       <c r="E70">
-        <v>-14.17793232</v>
+        <v>-0.24745160010891828</v>
       </c>
       <c r="F70">
-        <v>3.3282863699999998</v>
+        <v>5.8089555605750222E-2</v>
       </c>
       <c r="G70">
-        <f t="shared" si="4"/>
-        <v>4.78943355</v>
+        <v>8.359138475298046E-2</v>
       </c>
       <c r="H70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.0495893530064748E-3</v>
       </c>
     </row>
@@ -5918,23 +5853,22 @@
         <v>1.0429633599999999</v>
       </c>
       <c r="C71">
-        <v>6.0386766099999996</v>
+        <v>0.10539478930766952</v>
       </c>
       <c r="D71">
-        <v>1.8281445000000001</v>
+        <v>3.1907140727225475E-2</v>
       </c>
       <c r="E71">
-        <v>-13.1754494</v>
+        <v>-0.22995497245991137</v>
       </c>
       <c r="F71">
-        <v>3.7398007299999998</v>
+        <v>6.5271836106987474E-2</v>
       </c>
       <c r="G71">
-        <f t="shared" si="4"/>
-        <v>5.3086282899999997</v>
+        <v>9.265304242501636E-2</v>
       </c>
       <c r="H71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4.2587856066123031E-4</v>
       </c>
     </row>
@@ -5946,23 +5880,22 @@
         <v>1.0443779</v>
       </c>
       <c r="C72">
-        <v>6.0480910200000002</v>
+        <v>0.10555910175930222</v>
       </c>
       <c r="D72">
-        <v>0.16717893</v>
+        <v>2.9178227684611238E-3</v>
       </c>
       <c r="E72">
-        <v>-12.03988618</v>
+        <v>-0.21013565540636264</v>
       </c>
       <c r="F72">
-        <v>4.1774215000000003</v>
+        <v>7.2909759418600312E-2</v>
       </c>
       <c r="G72">
-        <f t="shared" si="4"/>
-        <v>5.8246162299999993</v>
+        <v>0.10165873087859929</v>
       </c>
       <c r="H72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3.872033836704869E-4</v>
       </c>
     </row>
@@ -5974,23 +5907,22 @@
         <v>1.0449949700000001</v>
       </c>
       <c r="C73">
-        <v>5.9788536700000003</v>
+        <v>0.10435068203644653</v>
       </c>
       <c r="D73">
-        <v>-1.2724690400000001</v>
+        <v>-2.2208774377691427E-2</v>
       </c>
       <c r="E73">
-        <v>-11.11751529</v>
+        <v>-0.19403724645131221</v>
       </c>
       <c r="F73">
-        <v>4.6742666100000001</v>
+        <v>8.158134246053371E-2</v>
       </c>
       <c r="G73">
-        <f t="shared" si="4"/>
-        <v>6.4111306599999995</v>
+        <v>0.1118953387925571</v>
       </c>
       <c r="H73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.1299940437380371E-4</v>
       </c>
     </row>
@@ -6002,23 +5934,22 @@
         <v>1.0453948099999999</v>
       </c>
       <c r="C74">
-        <v>5.9651296800000004</v>
+        <v>0.10411115322443575</v>
       </c>
       <c r="D74">
-        <v>-2.99510181</v>
+        <v>-5.2274388016941627E-2</v>
       </c>
       <c r="E74">
-        <v>-9.8454519099999995</v>
+        <v>-0.17183555217626442</v>
       </c>
       <c r="F74">
-        <v>5.0655643799999996</v>
+        <v>8.8410776902745195E-2</v>
       </c>
       <c r="G74">
-        <f t="shared" si="4"/>
-        <v>6.8754240399999986</v>
+        <v>0.1199987869687703</v>
       </c>
       <c r="H74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added stretch factor to sigmoid so [0, max] corresponds to [0, 1]
</commit_message>
<xml_diff>
--- a/BME 355/Project/data/data.xlsx
+++ b/BME 355/Project/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Uni-Projects\BME 355\Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79102C80-11A5-4847-A03E-DBC635180865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232ED157-22F8-4BF4-B2B7-92D505973BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -2397,6 +2397,869 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ankle Angle (Left)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ankle Angle</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$A$2:$A$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="73"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.699999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2999999999999974E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9999999999999989E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2999999999999963E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.9999999999999978E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.13300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.16699999999999993</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.18299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.19999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.21699999999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.23299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.26700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.28300000000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.29999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.31699999999999995</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.33299999999999996</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.36699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.38300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.41699999999999993</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.43299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.44999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.46699999999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.48299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.51700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.53300000000000003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.54999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.56699999999999995</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.58299999999999996</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.61699999999999988</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.6329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.66699999999999993</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.68299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.70000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.71699999999999997</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.73299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.74999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.76700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.78300000000000003</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.81700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.83300000000000007</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.86699999999999988</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.8829999999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.91699999999999993</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.93299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.95000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.96699999999999997</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.98299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.0169999999999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.0329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.0670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.0830000000000002</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.117</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.133</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.1669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.1829999999999998</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.2000000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$F$2:$F$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="73"/>
+                <c:pt idx="0">
+                  <c:v>9.4197304162127349E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8238263059407638E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1027846008911588</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10893767975658385</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11605902383231699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12196132349337288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12786532031259343</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.13527207057598939</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14518821387359954</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15313339524417602</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.16407847628381547</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.17941230780624723</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.18900873418656128</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.20158263572210985</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.21007824245155246</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.21554440911621034</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.21554977129127126</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.21053446209324581</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.19686143579606236</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.1748636722485358</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.14427311156684014</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.5814316458449206E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.2604226626735414E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-3.5505271196031266E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-9.4587321719963299E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.12929161227850239</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.13595856494493361</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.12006379821447907</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-9.4023916871048913E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-6.7366924628692482E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-4.4072507808772012E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-2.5342212503950051E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-1.1214929187817101E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-2.4517495214097822E-4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.7754777799156462E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.8541332520965809E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.4998155050372704E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.9207676625080139E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.8388201431636277E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.2130893597677233E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.2779872203899584E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-5.7722192247072225E-4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-1.2490222073627585E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-2.3146721473563107E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-2.8437826378258233E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-3.0339603628275751E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-2.6533639526675402E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-1.9536970951663395E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-1.322079263843581E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-7.4458671061904437E-3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-7.416713126365132E-3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-1.3850367806215205E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-2.7223921260096439E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-4.6636998094944843E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-6.143289872155968E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-7.0442241545530457E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-7.2102975212279388E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-6.7395540174443561E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-5.7910950129274184E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-4.516427077162196E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-2.8714690924561824E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-1.3497230102671435E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.9026155486538881E-4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.3981842411570385E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.6364026684637346E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.4775942956584607E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.4529557005458839E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5.1917153676577579E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5.8089555605750222E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.5271836106987474E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7.2909759418600312E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>8.158134246053371E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>8.8410776902745195E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1AE1-4369-8DB8-52A4598E36D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="786783320"/>
+        <c:axId val="786785944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="786783320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="786785944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="786785944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Height (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="786783320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2477,6 +3340,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2994,6 +3897,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3580,6 +4999,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>239059</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>119530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>721659</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>100480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784BFE76-1F55-488E-A053-5236BBDF58D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3888,8 +5345,8 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added start and stop vertical bars
</commit_message>
<xml_diff>
--- a/BME 355/Project/data/data.xlsx
+++ b/BME 355/Project/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Uni-Projects\BME 355\Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A5A734-5D29-45EB-94EB-3D6C0437D1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F66079-0DCC-4567-A09D-8C8E5457D747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3048,6 +3048,198 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Start</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="150"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>0.5</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-7A9B-487C-99AE-04C420A1FEEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>End</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="150"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>0.5</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-7A9B-487C-99AE-04C420A1FEEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -3180,6 +3372,8 @@
         <c:axId val="786785944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.25"/>
+          <c:min val="-0.2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3939,6 +4133,198 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Start</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="150"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>0.5</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AE64-45B1-AE8C-6AFF2FB503C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>End</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="150"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>0.5</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AE64-45B1-AE8C-6AFF2FB503C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -4071,6 +4457,8 @@
         <c:axId val="786785944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.14000000000000001"/>
+          <c:min val="-4.0000000000000008E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6914,9 +7302,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O66" sqref="O66"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q57" sqref="Q57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Changed reference ankle angle to degrees
</commit_message>
<xml_diff>
--- a/BME 355/Project/data/data.xlsx
+++ b/BME 355/Project/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Uni-Projects\BME 355\Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F66079-0DCC-4567-A09D-8C8E5457D747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38209839-5574-42DA-9F97-90E606A33D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>time</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>toe_height</t>
+  </si>
+  <si>
+    <t>ref_ankle_angle_l_degrees</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1036,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data!$G$2:$G$74</c:f>
+              <c:f>data!$H$2:$H$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="73"/>
@@ -1924,7 +1927,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data!$H$2:$H$74</c:f>
+              <c:f>data!$I$2:$I$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="73"/>
@@ -2815,228 +2818,228 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data!$F$2:$F$74</c:f>
+              <c:f>data!$G$2:$G$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="73"/>
                 <c:pt idx="0">
-                  <c:v>9.4197304162127349E-2</c:v>
+                  <c:v>5.3971079700000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.8238263059407638E-2</c:v>
+                  <c:v>5.6286378600000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1027846008911588</c:v>
+                  <c:v>5.8891238299999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10893767975658385</c:v>
+                  <c:v>6.24166928</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11605902383231699</c:v>
+                  <c:v>6.6496922400000011</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.12196132349337288</c:v>
+                  <c:v>6.9878690999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12786532031259343</c:v>
+                  <c:v>7.3261431999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.13527207057598939</c:v>
+                  <c:v>7.7505187299999987</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.14518821387359954</c:v>
+                  <c:v>8.3186718899999992</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.15313339524417602</c:v>
+                  <c:v>8.7738972499999992</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.16407847628381547</c:v>
+                  <c:v>9.4010041999999991</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.17941230780624723</c:v>
+                  <c:v>10.27956803</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.18900873418656128</c:v>
+                  <c:v>10.829402760000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.20158263572210985</c:v>
+                  <c:v>11.549834249999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.21007824245155246</c:v>
+                  <c:v>12.036596660000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.21554440911621034</c:v>
+                  <c:v>12.349784939999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.21554977129127126</c:v>
+                  <c:v>12.35009217</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.21053446209324581</c:v>
+                  <c:v>12.06273612</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.19686143579606236</c:v>
+                  <c:v>11.27932942</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.1748636722485358</c:v>
+                  <c:v>10.018950409999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.14427311156684014</c:v>
+                  <c:v>8.2662403900000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.5814316458449206E-2</c:v>
+                  <c:v>5.4897559500000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.2604226626735414E-2</c:v>
+                  <c:v>1.8680845800000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-3.5505271196031266E-2</c:v>
+                  <c:v>-2.03430219</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-9.4587321719963299E-2</c:v>
+                  <c:v>-5.4194543299999998</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.12929161227850239</c:v>
+                  <c:v>-7.40786371</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.13595856494493361</c:v>
+                  <c:v>-7.7898519599999991</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.12006379821447907</c:v>
+                  <c:v>-6.8791489099999996</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-9.4023916871048913E-2</c:v>
+                  <c:v>-5.3871736099999996</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-6.7366924628692482E-2</c:v>
+                  <c:v>-3.8598404599999996</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-4.4072507808772012E-2</c:v>
+                  <c:v>-2.5251686900000001</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-2.5342212503950051E-2</c:v>
+                  <c:v>-1.45200182</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-1.1214929187817101E-2</c:v>
+                  <c:v>-0.64256811000000003</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-2.4517495214097822E-4</c:v>
+                  <c:v>-1.4047489999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.7754777799156462E-3</c:v>
+                  <c:v>0.50279784000000005</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.8541332520965809E-2</c:v>
+                  <c:v>1.0623400999999999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.4998155050372704E-2</c:v>
+                  <c:v>1.4322887799999997</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.9207676625080139E-2</c:v>
+                  <c:v>1.6734766000000001</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.8388201431636277E-2</c:v>
+                  <c:v>1.6265241300000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.2130893597677233E-2</c:v>
+                  <c:v>1.2680068</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.2779872203899584E-2</c:v>
+                  <c:v>0.73223274000000005</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-5.7722192247072225E-4</c:v>
+                  <c:v>-3.3072379999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-1.2490222073627585E-2</c:v>
+                  <c:v>-0.71563701000000002</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-2.3146721473563107E-2</c:v>
+                  <c:v>-1.3262094499999997</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-2.8437826378258233E-2</c:v>
+                  <c:v>-1.6293674300000001</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-3.0339603628275751E-2</c:v>
+                  <c:v>-1.7383312399999999</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-2.6533639526675402E-2</c:v>
+                  <c:v>-1.5202655599999999</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-1.9536970951663395E-2</c:v>
+                  <c:v>-1.1193859799999999</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-1.322079263843581E-2</c:v>
+                  <c:v>-0.75749562000000004</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-7.4458671061904437E-3</c:v>
+                  <c:v>-0.42661675999999998</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-7.416713126365132E-3</c:v>
+                  <c:v>-0.42494636000000008</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-1.3850367806215205E-2</c:v>
+                  <c:v>-0.79356762000000003</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-2.7223921260096439E-2</c:v>
+                  <c:v>-1.5598157899999998</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-4.6636998094944843E-2</c:v>
+                  <c:v>-2.6721031600000003</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-6.143289872155968E-2</c:v>
+                  <c:v>-3.5198458200000005</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-7.0442241545530457E-2</c:v>
+                  <c:v>-4.0360431400000003</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-7.2102975212279388E-2</c:v>
+                  <c:v>-4.1311961699999999</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-6.7395540174443561E-2</c:v>
+                  <c:v>-3.8614800100000002</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-5.7910950129274184E-2</c:v>
+                  <c:v>-3.3180530299999997</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-4.516427077162196E-2</c:v>
+                  <c:v>-2.5877221000000001</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-2.8714690924561824E-2</c:v>
+                  <c:v>-1.6452306000000003</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-1.3497230102671435E-2</c:v>
+                  <c:v>-0.77333432000000002</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>3.9026155486538881E-4</c:v>
+                  <c:v>2.2360339999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.3981842411570385E-2</c:v>
+                  <c:v>0.80110055999999996</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2.6364026684637346E-2</c:v>
+                  <c:v>1.5105474600000002</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>3.4775942956584607E-2</c:v>
+                  <c:v>1.9925147599999999</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4.4529557005458839E-2</c:v>
+                  <c:v>2.5513556799999999</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>5.1917153676577579E-2</c:v>
+                  <c:v>2.9746337900000004</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.8089555605750222E-2</c:v>
+                  <c:v>3.3282863699999998</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>6.5271836106987474E-2</c:v>
+                  <c:v>3.7398007299999998</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>7.2909759418600312E-2</c:v>
+                  <c:v>4.1774215000000003</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>8.158134246053371E-2</c:v>
+                  <c:v>4.6742666100000001</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>8.8410776902745195E-2</c:v>
+                  <c:v>5.0655643799999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3118,7 +3121,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>data!$L$12</c:f>
+              <c:f>data!$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3133,7 +3136,7 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>0.5</c:v>
+                <c:v>90</c:v>
               </c:pt>
             </c:numLit>
           </c:yVal>
@@ -3214,7 +3217,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>data!$L$13</c:f>
+              <c:f>data!$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3229,7 +3232,7 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>0.5</c:v>
+                <c:v>90</c:v>
               </c:pt>
             </c:numLit>
           </c:yVal>
@@ -3372,8 +3375,8 @@
         <c:axId val="786785944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.25"/>
-          <c:min val="-0.2"/>
+          <c:max val="15"/>
+          <c:min val="-10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3412,7 +3415,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-CA"/>
-                  <a:t>Height (m)</a:t>
+                  <a:t>Angle (Degrees)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3900,7 +3903,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data!$I$2:$I$74</c:f>
+              <c:f>data!$J$2:$J$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="73"/>
@@ -4203,7 +4206,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>data!$L$12</c:f>
+              <c:f>data!$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -4299,7 +4302,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>data!$L$13</c:f>
+              <c:f>data!$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -6852,13 +6855,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>244475</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>727075</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -6888,13 +6891,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>711200</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -6926,14 +6929,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>239059</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>261470</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>119530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>179294</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>201705</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>100480</xdr:rowOff>
     </xdr:to>
@@ -6964,13 +6967,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>186765</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>179294</xdr:colOff>
       <xdr:row>77</xdr:row>
       <xdr:rowOff>107951</xdr:rowOff>
@@ -7300,16 +7303,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R74"/>
+  <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q57" sqref="Q57"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7329,20 +7332,23 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7362,24 +7368,28 @@
         <v>9.4197304162127349E-2</v>
       </c>
       <c r="G2">
+        <f>DEGREES(F2)</f>
+        <v>5.3971079700000004</v>
+      </c>
+      <c r="H2">
         <v>0.14509683541528215</v>
       </c>
-      <c r="H2">
-        <f>B2-$L$6*COS(C2+D2)-$L$7*COS(C2+D2+E2)-$L$10</f>
+      <c r="I2">
+        <f>B2-$M$6*COS(C2+D2)-$M$7*COS(C2+D2+E2)-$M$10</f>
         <v>7.116865845925302E-4</v>
       </c>
-      <c r="I2">
-        <f>H2+$L$8*SIN(F2-G2)</f>
+      <c r="J2">
+        <f>I2+$M$8*SIN(F2-H2)</f>
         <v>-8.6970189619925559E-3</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>1</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.1950308</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.699999999999996E-2</v>
       </c>
@@ -7399,24 +7409,28 @@
         <v>9.8238263059407638E-2</v>
       </c>
       <c r="G3">
+        <f>DEGREES(F3)</f>
+        <v>5.6286378600000004</v>
+      </c>
+      <c r="H3">
         <v>0.15378178209423221</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H66" si="0">B3-$L$6*COS(C3+D3)-$L$7*COS(C3+D3+E3)-$L$10</f>
+      <c r="I3">
+        <f>B3-$M$6*COS(C3+D3)-$M$7*COS(C3+D3+E3)-$M$10</f>
         <v>9.1260743201959649E-4</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I66" si="1">H3+$L$8*SIN(F3-G3)</f>
+      <c r="J3">
+        <f>I3+$M$8*SIN(F3-H3)</f>
         <v>-9.3536866122984896E-3</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>2</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.18455724409999999</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3.2999999999999974E-2</v>
       </c>
@@ -7436,25 +7450,29 @@
         <v>0.1027846008911588</v>
       </c>
       <c r="G4">
+        <f>DEGREES(F4)</f>
+        <v>5.8891238299999999</v>
+      </c>
+      <c r="H4">
         <v>0.16275075632526897</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
+      <c r="I4">
+        <f>B4-$M$6*COS(C4+D4)-$M$7*COS(C4+D4+E4)-$M$10</f>
         <v>8.6453401385977457E-4</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
+      <c r="J4">
+        <f>I4+$M$8*SIN(F4-H4)</f>
         <v>-1.0218266808236863E-2</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>3</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f>1.045</f>
         <v>1.0449999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4.9999999999999989E-2</v>
       </c>
@@ -7474,18 +7492,22 @@
         <v>0.10893767975658385</v>
       </c>
       <c r="G5">
+        <f>DEGREES(F5)</f>
+        <v>6.24166928</v>
+      </c>
+      <c r="H5">
         <v>0.17357485288648947</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
+      <c r="I5">
+        <f>B5-$M$6*COS(C5+D5)-$M$7*COS(C5+D5+E5)-$M$10</f>
         <v>1.1958020955685766E-3</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
+      <c r="J5">
+        <f>I5+$M$8*SIN(F5-H5)</f>
         <v>-1.0749125935231122E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6.7000000000000004E-2</v>
       </c>
@@ -7505,25 +7527,29 @@
         <v>0.11605902383231699</v>
       </c>
       <c r="G6">
+        <f>DEGREES(F6)</f>
+        <v>6.6496922400000011</v>
+      </c>
+      <c r="H6">
         <v>0.18558447760662936</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
+      <c r="I6">
+        <f>B6-$M$6*COS(C6+D6)-$M$7*COS(C6+D6+E6)-$M$10</f>
         <v>1.0083137324033431E-3</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
+      <c r="J6">
+        <f>I6+$M$8*SIN(F6-H6)</f>
         <v>-1.1838562215760838E-2</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>4</v>
       </c>
-      <c r="L6">
-        <f>L2/(L2+L3)*L4</f>
+      <c r="M6">
+        <f>M2/(M2+M3)*M4</f>
         <v>0.53691676850156089</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>8.2999999999999963E-2</v>
       </c>
@@ -7543,25 +7569,29 @@
         <v>0.12196132349337288</v>
       </c>
       <c r="G7">
+        <f>DEGREES(F7)</f>
+        <v>6.9878690999999993</v>
+      </c>
+      <c r="H7">
         <v>0.19659764603478422</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
+      <c r="I7">
+        <f>B7-$M$6*COS(C7+D7)-$M$7*COS(C7+D7+E7)-$M$10</f>
         <v>1.5440728229624834E-3</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
+      <c r="J7">
+        <f>I7+$M$8*SIN(F7-H7)</f>
         <v>-1.2245492674982993E-2</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>5</v>
       </c>
-      <c r="L7">
-        <f>L3/(L2+L3)*L4</f>
+      <c r="M7">
+        <f>M3/(M2+M3)*M4</f>
         <v>0.50808323149843904</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>9.9999999999999978E-2</v>
       </c>
@@ -7581,25 +7611,29 @@
         <v>0.12786532031259343</v>
       </c>
       <c r="G8">
+        <f>DEGREES(F8)</f>
+        <v>7.3261431999999997</v>
+      </c>
+      <c r="H8">
         <v>0.20872098419167934</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
+      <c r="I8">
+        <f>B8-$M$6*COS(C8+D8)-$M$7*COS(C8+D8+E8)-$M$10</f>
         <v>2.049032133853157E-3</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
+      <c r="J8">
+        <f>I8+$M$8*SIN(F8-H8)</f>
         <v>-1.2887190218280248E-2</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>16</v>
       </c>
-      <c r="L8">
-        <f>-H23/SIN(F23-G23)</f>
+      <c r="M8">
+        <f>-I23/SIN(F23-H23)</f>
         <v>0.18492841020407733</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.11699999999999999</v>
       </c>
@@ -7619,18 +7653,22 @@
         <v>0.13527207057598939</v>
       </c>
       <c r="G9">
+        <f>DEGREES(F9)</f>
+        <v>7.7505187299999987</v>
+      </c>
+      <c r="H9">
         <v>0.22290572793557817</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
+      <c r="I9">
+        <f>B9-$M$6*COS(C9+D9)-$M$7*COS(C9+D9+E9)-$M$10</f>
         <v>2.5035843062888308E-3</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
+      <c r="J9">
+        <f>I9+$M$8*SIN(F9-H9)</f>
         <v>-1.3681633897218427E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.13300000000000001</v>
       </c>
@@ -7650,24 +7688,28 @@
         <v>0.14518821387359954</v>
       </c>
       <c r="G10">
+        <f>DEGREES(F10)</f>
+        <v>8.3186718899999992</v>
+      </c>
+      <c r="H10">
         <v>0.23995935436851457</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
+      <c r="I10">
+        <f>B10-$M$6*COS(C10+D10)-$M$7*COS(C10+D10+E10)-$M$10</f>
         <v>3.1148040156381285E-3</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
+      <c r="J10">
+        <f>I10+$M$8*SIN(F10-H10)</f>
         <v>-1.4384849130205234E-2</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>13</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>4.7697474025435449E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.15000000000000002</v>
       </c>
@@ -7687,18 +7729,22 @@
         <v>0.15313339524417602</v>
       </c>
       <c r="G11">
+        <f>DEGREES(F11)</f>
+        <v>8.7738972499999992</v>
+      </c>
+      <c r="H11">
         <v>0.25726778805120093</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
+      <c r="I11">
+        <f>B11-$M$6*COS(C11+D11)-$M$7*COS(C11+D11+E11)-$M$10</f>
         <v>4.2889845957959638E-3</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
+      <c r="J11">
+        <f>I11+$M$8*SIN(F11-H11)</f>
         <v>-1.4933637515388381E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.16699999999999993</v>
       </c>
@@ -7718,24 +7764,28 @@
         <v>0.16407847628381547</v>
       </c>
       <c r="G12">
+        <f>DEGREES(F12)</f>
+        <v>9.4010041999999991</v>
+      </c>
+      <c r="H12">
         <v>0.27813175779136384</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
+      <c r="I12">
+        <f>B12-$M$6*COS(C12+D12)-$M$7*COS(C12+D12+E12)-$M$10</f>
         <v>5.9003631058472394E-3</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
+      <c r="J12">
+        <f>I12+$M$8*SIN(F12-H12)</f>
         <v>-1.5145631334882368E-2</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>14</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>0.35</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.18299999999999994</v>
       </c>
@@ -7755,24 +7805,28 @@
         <v>0.17941230780624723</v>
       </c>
       <c r="G13">
+        <f>DEGREES(F13)</f>
+        <v>10.27956803</v>
+      </c>
+      <c r="H13">
         <v>0.30551729758739249</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
+      <c r="I13">
+        <f>B13-$M$6*COS(C13+D13)-$M$7*COS(C13+D13+E13)-$M$10</f>
         <v>8.1924473549296883E-3</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
+      <c r="J13">
+        <f>I13+$M$8*SIN(F13-H13)</f>
         <v>-1.5066188409308318E-2</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>15</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0.95</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.19999999999999996</v>
       </c>
@@ -7792,18 +7846,22 @@
         <v>0.18900873418656128</v>
       </c>
       <c r="G14">
+        <f>DEGREES(F14)</f>
+        <v>10.829402760000001</v>
+      </c>
+      <c r="H14">
         <v>0.3327623568791257</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
+      <c r="I14">
+        <f>B14-$M$6*COS(C14+D14)-$M$7*COS(C14+D14+E14)-$M$10</f>
         <v>1.2297223767784748E-2</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
+      <c r="J14">
+        <f>I14+$M$8*SIN(F14-H14)</f>
         <v>-1.4195439065196182E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.21699999999999997</v>
       </c>
@@ -7823,18 +7881,22 @@
         <v>0.20158263572210985</v>
       </c>
       <c r="G15">
+        <f>DEGREES(F15)</f>
+        <v>11.549834249999998</v>
+      </c>
+      <c r="H15">
         <v>0.36492578280091165</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
+      <c r="I15">
+        <f>B15-$M$6*COS(C15+D15)-$M$7*COS(C15+D15+E15)-$M$10</f>
         <v>1.7191415794078901E-2</v>
       </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
+      <c r="J15">
+        <f>I15+$M$8*SIN(F15-H15)</f>
         <v>-1.2881227322641093E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.23299999999999998</v>
       </c>
@@ -7854,18 +7916,22 @@
         <v>0.21007824245155246</v>
       </c>
       <c r="G16">
+        <f>DEGREES(F16)</f>
+        <v>12.036596660000001</v>
+      </c>
+      <c r="H16">
         <v>0.39971119329602367</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
+      <c r="I16">
+        <f>B16-$M$6*COS(C16+D16)-$M$7*COS(C16+D16+E16)-$M$10</f>
         <v>2.3410577379752273E-2</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
+      <c r="J16">
+        <f>I16+$M$8*SIN(F16-H16)</f>
         <v>-1.1448139166418667E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.25</v>
       </c>
@@ -7885,18 +7951,22 @@
         <v>0.21554440911621034</v>
       </c>
       <c r="G17">
+        <f>DEGREES(F17)</f>
+        <v>12.349784939999999</v>
+      </c>
+      <c r="H17">
         <v>0.43620564590265176</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
+      <c r="I17">
+        <f>B17-$M$6*COS(C17+D17)-$M$7*COS(C17+D17+E17)-$M$10</f>
         <v>3.0533244046068053E-2</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
+      <c r="J17">
+        <f>I17+$M$8*SIN(F17-H17)</f>
         <v>-9.942938550733714E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.26700000000000002</v>
       </c>
@@ -7916,18 +7986,22 @@
         <v>0.21554977129127126</v>
       </c>
       <c r="G18">
+        <f>DEGREES(F18)</f>
+        <v>12.35009217</v>
+      </c>
+      <c r="H18">
         <v>0.47635212509445313</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="0"/>
+      <c r="I18">
+        <f>B18-$M$6*COS(C18+D18)-$M$7*COS(C18+D18+E18)-$M$10</f>
         <v>3.9180989531838406E-2</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="1"/>
+      <c r="J18">
+        <f>I18+$M$8*SIN(F18-H18)</f>
         <v>-8.5038839306207717E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0.28300000000000003</v>
       </c>
@@ -7947,18 +8021,22 @@
         <v>0.21053446209324581</v>
       </c>
       <c r="G19">
+        <f>DEGREES(F19)</f>
+        <v>12.06273612</v>
+      </c>
+      <c r="H19">
         <v>0.52186067375473699</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
+      <c r="I19">
+        <f>B19-$M$6*COS(C19+D19)-$M$7*COS(C19+D19+E19)-$M$10</f>
         <v>4.9623117916908099E-2</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="1"/>
+      <c r="J19">
+        <f>I19+$M$8*SIN(F19-H19)</f>
         <v>-7.024404880903147E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0.29999999999999993</v>
       </c>
@@ -7978,18 +8056,22 @@
         <v>0.19686143579606236</v>
       </c>
       <c r="G20">
+        <f>DEGREES(F20)</f>
+        <v>11.27932942</v>
+      </c>
+      <c r="H20">
         <v>0.57283033216270407</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="0"/>
+      <c r="I20">
+        <f>B20-$M$6*COS(C20+D20)-$M$7*COS(C20+D20+E20)-$M$10</f>
         <v>6.2844480971263994E-2</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
+      <c r="J20">
+        <f>I20+$M$8*SIN(F20-H20)</f>
         <v>-5.056408780982985E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0.31699999999999995</v>
       </c>
@@ -8009,18 +8091,22 @@
         <v>0.1748636722485358</v>
       </c>
       <c r="G21">
+        <f>DEGREES(F21)</f>
+        <v>10.018950409999999</v>
+      </c>
+      <c r="H21">
         <v>0.63028875803591011</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="0"/>
+      <c r="I21">
+        <f>B21-$M$6*COS(C21+D21)-$M$7*COS(C21+D21+E21)-$M$10</f>
         <v>7.8032151444156983E-2</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="1"/>
+      <c r="J21">
+        <f>I21+$M$8*SIN(F21-H21)</f>
         <v>-3.3075209414978463E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.33299999999999996</v>
       </c>
@@ -8040,18 +8126,22 @@
         <v>0.14427311156684014</v>
       </c>
       <c r="G22">
+        <f>DEGREES(F22)</f>
+        <v>8.2662403900000001</v>
+      </c>
+      <c r="H22">
         <v>0.69752678608508545</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="0"/>
+      <c r="I22">
+        <f>B22-$M$6*COS(C22+D22)-$M$7*COS(C22+D22+E22)-$M$10</f>
         <v>9.5443317830569585E-2</v>
       </c>
-      <c r="I22">
-        <f t="shared" si="1"/>
+      <c r="J22">
+        <f>I22+$M$8*SIN(F22-H22)</f>
         <v>-1.7288492303865755E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0.35</v>
       </c>
@@ -8071,18 +8161,22 @@
         <v>9.5814316458449206E-2</v>
       </c>
       <c r="G23">
+        <f>DEGREES(F23)</f>
+        <v>5.4897559500000002</v>
+      </c>
+      <c r="H23">
         <v>0.76355485956886104</v>
       </c>
-      <c r="H23">
-        <f t="shared" si="0"/>
+      <c r="I23">
+        <f>B23-$M$6*COS(C23+D23)-$M$7*COS(C23+D23+E23)-$M$10</f>
         <v>0.1145101481908945</v>
       </c>
-      <c r="I23">
-        <f t="shared" si="1"/>
+      <c r="J23">
+        <f>I23+$M$8*SIN(F23-H23)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.36699999999999999</v>
       </c>
@@ -8102,18 +8196,22 @@
         <v>3.2604226626735414E-2</v>
       </c>
       <c r="G24">
+        <f>DEGREES(F24)</f>
+        <v>1.8680845800000001</v>
+      </c>
+      <c r="H24">
         <v>0.82706138955976882</v>
       </c>
-      <c r="H24">
-        <f t="shared" si="0"/>
+      <c r="I24">
+        <f>B24-$M$6*COS(C24+D24)-$M$7*COS(C24+D24+E24)-$M$10</f>
         <v>0.13423640324778313</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="1"/>
+      <c r="J24">
+        <f>I24+$M$8*SIN(F24-H24)</f>
         <v>2.2930599150908504E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.38300000000000001</v>
       </c>
@@ -8133,18 +8231,22 @@
         <v>-3.5505271196031266E-2</v>
       </c>
       <c r="G25">
+        <f>DEGREES(F25)</f>
+        <v>-2.03430219</v>
+      </c>
+      <c r="H25">
         <v>0.88179699289131819</v>
       </c>
-      <c r="H25">
-        <f t="shared" si="0"/>
+      <c r="I25">
+        <f>B25-$M$6*COS(C25+D25)-$M$7*COS(C25+D25+E25)-$M$10</f>
         <v>0.15323679456369976</v>
       </c>
-      <c r="I25">
-        <f t="shared" si="1"/>
+      <c r="J25">
+        <f>I25+$M$8*SIN(F25-H25)</f>
         <v>6.4102232495565903E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.4</v>
       </c>
@@ -8164,18 +8266,22 @@
         <v>-9.4587321719963299E-2</v>
       </c>
       <c r="G26">
+        <f>DEGREES(F26)</f>
+        <v>-5.4194543299999998</v>
+      </c>
+      <c r="H26">
         <v>0.92732326414842581</v>
       </c>
-      <c r="H26">
-        <f t="shared" si="0"/>
+      <c r="I26">
+        <f>B26-$M$6*COS(C26+D26)-$M$7*COS(C26+D26+E26)-$M$10</f>
         <v>0.17130633826703734</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="1"/>
+      <c r="J26">
+        <f>I26+$M$8*SIN(F26-H26)</f>
         <v>1.3542727667465726E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0.41699999999999993</v>
       </c>
@@ -8195,18 +8301,22 @@
         <v>-0.12929161227850239</v>
       </c>
       <c r="G27">
+        <f>DEGREES(F27)</f>
+        <v>-7.40786371</v>
+      </c>
+      <c r="H27">
         <v>0.96038131146179773</v>
       </c>
-      <c r="H27">
-        <f t="shared" si="0"/>
+      <c r="I27">
+        <f>B27-$M$6*COS(C27+D27)-$M$7*COS(C27+D27+E27)-$M$10</f>
         <v>0.18718269341486676</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="1"/>
+      <c r="J27">
+        <f>I27+$M$8*SIN(F27-H27)</f>
         <v>2.3248170199129503E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.43299999999999994</v>
       </c>
@@ -8226,18 +8336,22 @@
         <v>-0.13595856494493361</v>
       </c>
       <c r="G28">
+        <f>DEGREES(F28)</f>
+        <v>-7.7898519599999991</v>
+      </c>
+      <c r="H28">
         <v>0.98249849671993095</v>
       </c>
-      <c r="H28">
-        <f t="shared" si="0"/>
+      <c r="I28">
+        <f>B28-$M$6*COS(C28+D28)-$M$7*COS(C28+D28+E28)-$M$10</f>
         <v>0.20054261109685678</v>
       </c>
-      <c r="I28">
-        <f t="shared" si="1"/>
+      <c r="J28">
+        <f>I28+$M$8*SIN(F28-H28)</f>
         <v>3.4212980024603434E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0.44999999999999996</v>
       </c>
@@ -8257,18 +8371,22 @@
         <v>-0.12006379821447907</v>
       </c>
       <c r="G29">
+        <f>DEGREES(F29)</f>
+        <v>-6.8791489099999996</v>
+      </c>
+      <c r="H29">
         <v>0.99374180426325387</v>
       </c>
-      <c r="H29">
-        <f t="shared" si="0"/>
+      <c r="I29">
+        <f>B29-$M$6*COS(C29+D29)-$M$7*COS(C29+D29+E29)-$M$10</f>
         <v>0.21090315205236626</v>
       </c>
-      <c r="I29">
-        <f t="shared" si="1"/>
+      <c r="J29">
+        <f>I29+$M$8*SIN(F29-H29)</f>
         <v>4.4951281517514097E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0.46699999999999997</v>
       </c>
@@ -8288,18 +8406,22 @@
         <v>-9.4023916871048913E-2</v>
       </c>
       <c r="G30">
+        <f>DEGREES(F30)</f>
+        <v>-5.3871736099999996</v>
+      </c>
+      <c r="H30">
         <v>0.9929647742554879</v>
       </c>
-      <c r="H30">
-        <f t="shared" si="0"/>
+      <c r="I30">
+        <f>B30-$M$6*COS(C30+D30)-$M$7*COS(C30+D30+E30)-$M$10</f>
         <v>0.2172766258325512</v>
       </c>
-      <c r="I30">
-        <f t="shared" si="1"/>
+      <c r="J30">
+        <f>I30+$M$8*SIN(F30-H30)</f>
         <v>5.3572410375274326E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0.48299999999999998</v>
       </c>
@@ -8319,18 +8441,22 @@
         <v>-6.7366924628692482E-2</v>
       </c>
       <c r="G31">
+        <f>DEGREES(F31)</f>
+        <v>-3.8598404599999996</v>
+      </c>
+      <c r="H31">
         <v>0.97943821598913172</v>
       </c>
-      <c r="H31">
-        <f t="shared" si="0"/>
+      <c r="I31">
+        <f>B31-$M$6*COS(C31+D31)-$M$7*COS(C31+D31+E31)-$M$10</f>
         <v>0.2190479609110052</v>
       </c>
-      <c r="I31">
-        <f t="shared" si="1"/>
+      <c r="J31">
+        <f>I31+$M$8*SIN(F31-H31)</f>
         <v>5.8931556054755307E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0.5</v>
       </c>
@@ -8350,18 +8476,22 @@
         <v>-4.4072507808772012E-2</v>
       </c>
       <c r="G32">
+        <f>DEGREES(F32)</f>
+        <v>-2.5251686900000001</v>
+      </c>
+      <c r="H32">
         <v>0.95524670394794353</v>
       </c>
-      <c r="H32">
-        <f t="shared" si="0"/>
+      <c r="I32">
+        <f>B32-$M$6*COS(C32+D32)-$M$7*COS(C32+D32+E32)-$M$10</f>
         <v>0.21682194449721626</v>
       </c>
-      <c r="I32">
-        <f t="shared" si="1"/>
+      <c r="J32">
+        <f>I32+$M$8*SIN(F32-H32)</f>
         <v>6.1278111586190398E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0.51700000000000002</v>
       </c>
@@ -8381,18 +8511,22 @@
         <v>-2.5342212503950051E-2</v>
       </c>
       <c r="G33">
+        <f>DEGREES(F33)</f>
+        <v>-1.45200182</v>
+      </c>
+      <c r="H33">
         <v>0.91897405319317937</v>
       </c>
-      <c r="H33">
-        <f t="shared" si="0"/>
+      <c r="I33">
+        <f>B33-$M$6*COS(C33+D33)-$M$7*COS(C33+D33+E33)-$M$10</f>
         <v>0.20988608432065936</v>
       </c>
-      <c r="I33">
-        <f t="shared" si="1"/>
+      <c r="J33">
+        <f>I33+$M$8*SIN(F33-H33)</f>
         <v>6.0076272350184839E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0.53300000000000003</v>
       </c>
@@ -8412,18 +8546,22 @@
         <v>-1.1214929187817101E-2</v>
       </c>
       <c r="G34">
+        <f>DEGREES(F34)</f>
+        <v>-0.64256811000000003</v>
+      </c>
+      <c r="H34">
         <v>0.87193782848513357</v>
       </c>
-      <c r="H34">
-        <f t="shared" si="0"/>
+      <c r="I34">
+        <f>B34-$M$6*COS(C34+D34)-$M$7*COS(C34+D34+E34)-$M$10</f>
         <v>0.19892088731401658</v>
       </c>
-      <c r="I34">
-        <f t="shared" si="1"/>
+      <c r="J34">
+        <f>I34+$M$8*SIN(F34-H34)</f>
         <v>5.601859966874756E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>0.54999999999999993</v>
       </c>
@@ -8443,18 +8581,22 @@
         <v>-2.4517495214097822E-4</v>
       </c>
       <c r="G35">
+        <f>DEGREES(F35)</f>
+        <v>-1.4047489999999999E-2</v>
+      </c>
+      <c r="H35">
         <v>0.81566122561137777</v>
       </c>
-      <c r="H35">
-        <f t="shared" si="0"/>
+      <c r="I35">
+        <f>B35-$M$6*COS(C35+D35)-$M$7*COS(C35+D35+E35)-$M$10</f>
         <v>0.18411312598422808</v>
       </c>
-      <c r="I35">
-        <f t="shared" si="1"/>
+      <c r="J35">
+        <f>I35+$M$8*SIN(F35-H35)</f>
         <v>4.9421078546015629E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>0.56699999999999995</v>
       </c>
@@ -8474,18 +8616,22 @@
         <v>8.7754777799156462E-3</v>
       </c>
       <c r="G36">
+        <f>DEGREES(F36)</f>
+        <v>0.50279784000000005</v>
+      </c>
+      <c r="H36">
         <v>0.75015399520284476</v>
       </c>
-      <c r="H36">
-        <f t="shared" si="0"/>
+      <c r="I36">
+        <f>B36-$M$6*COS(C36+D36)-$M$7*COS(C36+D36+E36)-$M$10</f>
         <v>0.1667741547718396</v>
       </c>
-      <c r="I36">
-        <f t="shared" si="1"/>
+      <c r="J36">
+        <f>I36+$M$8*SIN(F36-H36)</f>
         <v>4.1891026193354011E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>0.58299999999999996</v>
       </c>
@@ -8505,18 +8651,22 @@
         <v>1.8541332520965809E-2</v>
       </c>
       <c r="G37">
+        <f>DEGREES(F37)</f>
+        <v>1.0623400999999999</v>
+      </c>
+      <c r="H37">
         <v>0.67779935590426521</v>
       </c>
-      <c r="H37">
-        <f t="shared" si="0"/>
+      <c r="I37">
+        <f>B37-$M$6*COS(C37+D37)-$M$7*COS(C37+D37+E37)-$M$10</f>
         <v>0.1477907798464192</v>
       </c>
-      <c r="I37">
-        <f t="shared" si="1"/>
+      <c r="J37">
+        <f>I37+$M$8*SIN(F37-H37)</f>
         <v>3.4516483195362699E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>0.6</v>
       </c>
@@ -8536,18 +8686,22 @@
         <v>2.4998155050372704E-2</v>
       </c>
       <c r="G38">
+        <f>DEGREES(F38)</f>
+        <v>1.4322887799999997</v>
+      </c>
+      <c r="H38">
         <v>0.59602230461325068</v>
       </c>
-      <c r="H38">
-        <f t="shared" si="0"/>
+      <c r="I38">
+        <f>B38-$M$6*COS(C38+D38)-$M$7*COS(C38+D38+E38)-$M$10</f>
         <v>0.12739154148061127</v>
       </c>
-      <c r="I38">
-        <f t="shared" si="1"/>
+      <c r="J38">
+        <f>I38+$M$8*SIN(F38-H38)</f>
         <v>2.7438845688297103E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>0.61699999999999988</v>
       </c>
@@ -8567,18 +8721,22 @@
         <v>2.9207676625080139E-2</v>
       </c>
       <c r="G39">
+        <f>DEGREES(F39)</f>
+        <v>1.6734766000000001</v>
+      </c>
+      <c r="H39">
         <v>0.50870245204264997</v>
       </c>
-      <c r="H39">
-        <f t="shared" si="0"/>
+      <c r="I39">
+        <f>B39-$M$6*COS(C39+D39)-$M$7*COS(C39+D39+E39)-$M$10</f>
         <v>0.10688229884476691</v>
       </c>
-      <c r="I39">
-        <f t="shared" si="1"/>
+      <c r="J39">
+        <f>I39+$M$8*SIN(F39-H39)</f>
         <v>2.156909321341216E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>0.6329999999999999</v>
       </c>
@@ -8598,18 +8756,22 @@
         <v>2.8388201431636277E-2</v>
       </c>
       <c r="G40">
+        <f>DEGREES(F40)</f>
+        <v>1.6265241300000002</v>
+      </c>
+      <c r="H40">
         <v>0.41624591065306188</v>
       </c>
-      <c r="H40">
-        <f t="shared" si="0"/>
+      <c r="I40">
+        <f>B40-$M$6*COS(C40+D40)-$M$7*COS(C40+D40+E40)-$M$10</f>
         <v>8.7505283312476922E-2</v>
       </c>
-      <c r="I40">
-        <f t="shared" si="1"/>
+      <c r="J40">
+        <f>I40+$M$8*SIN(F40-H40)</f>
         <v>1.7564226798678848E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>0.65</v>
       </c>
@@ -8629,18 +8791,22 @@
         <v>2.2130893597677233E-2</v>
       </c>
       <c r="G41">
+        <f>DEGREES(F41)</f>
+        <v>1.2680068</v>
+      </c>
+      <c r="H41">
         <v>0.31921897870023525</v>
       </c>
-      <c r="H41">
-        <f t="shared" si="0"/>
+      <c r="I41">
+        <f>B41-$M$6*COS(C41+D41)-$M$7*COS(C41+D41+E41)-$M$10</f>
         <v>7.025016139349255E-2</v>
       </c>
-      <c r="I41">
-        <f t="shared" si="1"/>
+      <c r="J41">
+        <f>I41+$M$8*SIN(F41-H41)</f>
         <v>1.611475504100264E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>0.66699999999999993</v>
       </c>
@@ -8660,18 +8826,22 @@
         <v>1.2779872203899584E-2</v>
       </c>
       <c r="G42">
+        <f>DEGREES(F42)</f>
+        <v>0.73223274000000005</v>
+      </c>
+      <c r="H42">
         <v>0.22058584763846742</v>
       </c>
-      <c r="H42">
-        <f t="shared" si="0"/>
+      <c r="I42">
+        <f>B42-$M$6*COS(C42+D42)-$M$7*COS(C42+D42+E42)-$M$10</f>
         <v>5.5769063846833167E-2</v>
       </c>
-      <c r="I42">
-        <f t="shared" si="1"/>
+      <c r="J42">
+        <f>I42+$M$8*SIN(F42-H42)</f>
         <v>1.7615822237529055E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>0.68299999999999994</v>
       </c>
@@ -8691,18 +8861,22 @@
         <v>-5.7722192247072225E-4</v>
       </c>
       <c r="G43">
+        <f>DEGREES(F43)</f>
+        <v>-3.3072379999999998E-2</v>
+      </c>
+      <c r="H43">
         <v>0.11987915424785699</v>
       </c>
-      <c r="H43">
-        <f t="shared" si="0"/>
+      <c r="I43">
+        <f>B43-$M$6*COS(C43+D43)-$M$7*COS(C43+D43+E43)-$M$10</f>
         <v>4.4631769934232235E-2</v>
       </c>
-      <c r="I43">
-        <f t="shared" si="1"/>
+      <c r="J43">
+        <f>I43+$M$8*SIN(F43-H43)</f>
         <v>2.2409794075990325E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>0.70000000000000007</v>
       </c>
@@ -8722,18 +8896,22 @@
         <v>-1.2490222073627585E-2</v>
       </c>
       <c r="G44">
+        <f>DEGREES(F44)</f>
+        <v>-0.71563701000000002</v>
+      </c>
+      <c r="H44">
         <v>2.2473019844437205E-2</v>
       </c>
-      <c r="H44">
-        <f t="shared" si="0"/>
+      <c r="I44">
+        <f>B44-$M$6*COS(C44+D44)-$M$7*COS(C44+D44+E44)-$M$10</f>
         <v>3.8066434157436269E-2</v>
       </c>
-      <c r="I44">
-        <f t="shared" si="1"/>
+      <c r="J44">
+        <f>I44+$M$8*SIN(F44-H44)</f>
         <v>3.1602054641865281E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>0.71699999999999997</v>
       </c>
@@ -8753,18 +8931,22 @@
         <v>-2.3146721473563107E-2</v>
       </c>
       <c r="G45">
+        <f>DEGREES(F45)</f>
+        <v>-1.3262094499999997</v>
+      </c>
+      <c r="H45">
         <v>-7.3909620324357217E-2</v>
       </c>
-      <c r="H45">
-        <f t="shared" si="0"/>
+      <c r="I45">
+        <f>B45-$M$6*COS(C45+D45)-$M$7*COS(C45+D45+E45)-$M$10</f>
         <v>3.5350444430718553E-2</v>
       </c>
-      <c r="I45">
-        <f t="shared" si="1"/>
+      <c r="J45">
+        <f>I45+$M$8*SIN(F45-H45)</f>
         <v>4.4733915400213722E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>0.73299999999999998</v>
       </c>
@@ -8784,18 +8966,22 @@
         <v>-2.8437826378258233E-2</v>
       </c>
       <c r="G46">
+        <f>DEGREES(F46)</f>
+        <v>-1.6293674300000001</v>
+      </c>
+      <c r="H46">
         <v>-0.16309002407178005</v>
       </c>
-      <c r="H46">
-        <f t="shared" si="0"/>
+      <c r="I46">
+        <f>B46-$M$6*COS(C46+D46)-$M$7*COS(C46+D46+E46)-$M$10</f>
         <v>3.6476976040728082E-2</v>
       </c>
-      <c r="I46">
-        <f t="shared" si="1"/>
+      <c r="J46">
+        <f>I46+$M$8*SIN(F46-H46)</f>
         <v>6.1302813465450495E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>0.74999999999999989</v>
       </c>
@@ -8815,18 +9001,22 @@
         <v>-3.0339603628275751E-2</v>
       </c>
       <c r="G47">
+        <f>DEGREES(F47)</f>
+        <v>-1.7383312399999999</v>
+      </c>
+      <c r="H47">
         <v>-0.24531907235489581</v>
       </c>
-      <c r="H47">
-        <f t="shared" si="0"/>
+      <c r="I47">
+        <f>B47-$M$6*COS(C47+D47)-$M$7*COS(C47+D47+E47)-$M$10</f>
         <v>4.020957671277603E-2</v>
       </c>
-      <c r="I47">
-        <f t="shared" si="1"/>
+      <c r="J47">
+        <f>I47+$M$8*SIN(F47-H47)</f>
         <v>7.965986804189612E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>0.76700000000000002</v>
       </c>
@@ -8846,18 +9036,22 @@
         <v>-2.6533639526675402E-2</v>
       </c>
       <c r="G48">
+        <f>DEGREES(F48)</f>
+        <v>-1.5202655599999999</v>
+      </c>
+      <c r="H48">
         <v>-0.31200130501616263</v>
       </c>
-      <c r="H48">
-        <f t="shared" si="0"/>
+      <c r="I48">
+        <f>B48-$M$6*COS(C48+D48)-$M$7*COS(C48+D48+E48)-$M$10</f>
         <v>4.4721659343532338E-2</v>
       </c>
-      <c r="I48">
-        <f t="shared" si="1"/>
+      <c r="J48">
+        <f>I48+$M$8*SIN(F48-H48)</f>
         <v>9.6798650127958394E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>0.78300000000000003</v>
       </c>
@@ -8877,18 +9071,22 @@
         <v>-1.9536970951663395E-2</v>
       </c>
       <c r="G49">
+        <f>DEGREES(F49)</f>
+        <v>-1.1193859799999999</v>
+      </c>
+      <c r="H49">
         <v>-0.36030995451045933</v>
       </c>
-      <c r="H49">
-        <f t="shared" si="0"/>
+      <c r="I49">
+        <f>B49-$M$6*COS(C49+D49)-$M$7*COS(C49+D49+E49)-$M$10</f>
         <v>4.8687397744538286E-2</v>
       </c>
-      <c r="I49">
-        <f t="shared" si="1"/>
+      <c r="J49">
+        <f>I49+$M$8*SIN(F49-H49)</f>
         <v>0.1104933806734394</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>0.79999999999999993</v>
       </c>
@@ -8908,18 +9106,22 @@
         <v>-1.322079263843581E-2</v>
       </c>
       <c r="G50">
+        <f>DEGREES(F50)</f>
+        <v>-0.75749562000000004</v>
+      </c>
+      <c r="H50">
         <v>-0.38966806228549938</v>
       </c>
-      <c r="H50">
-        <f t="shared" si="0"/>
+      <c r="I50">
+        <f>B50-$M$6*COS(C50+D50)-$M$7*COS(C50+D50+E50)-$M$10</f>
         <v>5.0434615952563155E-2</v>
       </c>
-      <c r="I50">
-        <f t="shared" si="1"/>
+      <c r="J50">
+        <f>I50+$M$8*SIN(F50-H50)</f>
         <v>0.11841778367957485</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>0.81700000000000006</v>
       </c>
@@ -8939,18 +9141,22 @@
         <v>-7.4458671061904437E-3</v>
       </c>
       <c r="G51">
+        <f>DEGREES(F51)</f>
+        <v>-0.42661675999999998</v>
+      </c>
+      <c r="H51">
         <v>-0.39539254117011097</v>
       </c>
-      <c r="H51">
-        <f t="shared" si="0"/>
+      <c r="I51">
+        <f>B51-$M$6*COS(C51+D51)-$M$7*COS(C51+D51+E51)-$M$10</f>
         <v>5.0014480836572339E-2</v>
       </c>
-      <c r="I51">
-        <f t="shared" si="1"/>
+      <c r="J51">
+        <f>I51+$M$8*SIN(F51-H51)</f>
         <v>0.11997076715968268</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>0.83300000000000007</v>
       </c>
@@ -8970,18 +9176,22 @@
         <v>-7.416713126365132E-3</v>
       </c>
       <c r="G52">
+        <f>DEGREES(F52)</f>
+        <v>-0.42494636000000008</v>
+      </c>
+      <c r="H52">
         <v>-0.38206282166039351</v>
       </c>
-      <c r="H52">
-        <f t="shared" si="0"/>
+      <c r="I52">
+        <f>B52-$M$6*COS(C52+D52)-$M$7*COS(C52+D52+E52)-$M$10</f>
         <v>4.6484928838822326E-2</v>
       </c>
-      <c r="I52">
-        <f t="shared" si="1"/>
+      <c r="J52">
+        <f>I52+$M$8*SIN(F52-H52)</f>
         <v>0.11415822441765583</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>0.85</v>
       </c>
@@ -9001,18 +9211,22 @@
         <v>-1.3850367806215205E-2</v>
       </c>
       <c r="G53">
+        <f>DEGREES(F53)</f>
+        <v>-0.79356762000000003</v>
+      </c>
+      <c r="H53">
         <v>-0.35289853252425457</v>
       </c>
-      <c r="H53">
-        <f t="shared" si="0"/>
+      <c r="I53">
+        <f>B53-$M$6*COS(C53+D53)-$M$7*COS(C53+D53+E53)-$M$10</f>
         <v>4.049533381557141E-2</v>
       </c>
-      <c r="I53">
-        <f t="shared" si="1"/>
+      <c r="J53">
+        <f>I53+$M$8*SIN(F53-H53)</f>
         <v>0.1020005986946538</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>0.86699999999999988</v>
       </c>
@@ -9032,18 +9246,22 @@
         <v>-2.7223921260096439E-2</v>
       </c>
       <c r="G54">
+        <f>DEGREES(F54)</f>
+        <v>-1.5598157899999998</v>
+      </c>
+      <c r="H54">
         <v>-0.31510553121766477</v>
       </c>
-      <c r="H54">
-        <f t="shared" si="0"/>
+      <c r="I54">
+        <f>B54-$M$6*COS(C54+D54)-$M$7*COS(C54+D54+E54)-$M$10</f>
         <v>3.4418892845651972E-2</v>
       </c>
-      <c r="I54">
-        <f t="shared" si="1"/>
+      <c r="J54">
+        <f>I54+$M$8*SIN(F54-H54)</f>
         <v>8.6924072336372032E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>0.8829999999999999</v>
       </c>
@@ -9063,18 +9281,22 @@
         <v>-4.6636998094944843E-2</v>
       </c>
       <c r="G55">
+        <f>DEGREES(F55)</f>
+        <v>-2.6721031600000003</v>
+      </c>
+      <c r="H55">
         <v>-0.27630546463523165</v>
       </c>
-      <c r="H55">
-        <f t="shared" si="0"/>
+      <c r="I55">
+        <f>B55-$M$6*COS(C55+D55)-$M$7*COS(C55+D55+E55)-$M$10</f>
         <v>2.904018514359763E-2</v>
       </c>
-      <c r="I55">
-        <f t="shared" si="1"/>
+      <c r="J55">
+        <f>I55+$M$8*SIN(F55-H55)</f>
         <v>7.1140008373865957E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>0.9</v>
       </c>
@@ -9094,18 +9316,22 @@
         <v>-6.143289872155968E-2</v>
       </c>
       <c r="G56">
+        <f>DEGREES(F56)</f>
+        <v>-3.5198458200000005</v>
+      </c>
+      <c r="H56">
         <v>-0.23416933400716755</v>
       </c>
-      <c r="H56">
-        <f t="shared" si="0"/>
+      <c r="I56">
+        <f>B56-$M$6*COS(C56+D56)-$M$7*COS(C56+D56+E56)-$M$10</f>
         <v>2.4333977182246114E-2</v>
       </c>
-      <c r="I56">
-        <f t="shared" si="1"/>
+      <c r="J56">
+        <f>I56+$M$8*SIN(F56-H56)</f>
         <v>5.611923214482821E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>0.91699999999999993</v>
       </c>
@@ -9125,18 +9351,22 @@
         <v>-7.0442241545530457E-2</v>
       </c>
       <c r="G57">
+        <f>DEGREES(F57)</f>
+        <v>-4.0360431400000003</v>
+      </c>
+      <c r="H57">
         <v>-0.1924718154411709</v>
       </c>
-      <c r="H57">
-        <f t="shared" si="0"/>
+      <c r="I57">
+        <f>B57-$M$6*COS(C57+D57)-$M$7*COS(C57+D57+E57)-$M$10</f>
         <v>2.0673792478827779E-2</v>
       </c>
-      <c r="I57">
-        <f t="shared" si="1"/>
+      <c r="J57">
+        <f>I57+$M$8*SIN(F57-H57)</f>
         <v>4.3184561572382679E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>0.93299999999999994</v>
       </c>
@@ -9156,18 +9386,22 @@
         <v>-7.2102975212279388E-2</v>
       </c>
       <c r="G58">
+        <f>DEGREES(F58)</f>
+        <v>-4.1311961699999999</v>
+      </c>
+      <c r="H58">
         <v>-0.15192429519197789</v>
       </c>
-      <c r="H58">
-        <f t="shared" si="0"/>
+      <c r="I58">
+        <f>B58-$M$6*COS(C58+D58)-$M$7*COS(C58+D58+E58)-$M$10</f>
         <v>1.782202706937297E-2</v>
       </c>
-      <c r="I58">
-        <f t="shared" si="1"/>
+      <c r="J58">
+        <f>I58+$M$8*SIN(F58-H58)</f>
         <v>3.256758681046721E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>0.95000000000000007</v>
       </c>
@@ -9187,18 +9421,22 @@
         <v>-6.7395540174443561E-2</v>
       </c>
       <c r="G59">
+        <f>DEGREES(F59)</f>
+        <v>-3.8614800100000002</v>
+      </c>
+      <c r="H59">
         <v>-0.11377327344872898</v>
       </c>
-      <c r="H59">
-        <f t="shared" si="0"/>
+      <c r="I59">
+        <f>B59-$M$6*COS(C59+D59)-$M$7*COS(C59+D59+E59)-$M$10</f>
         <v>1.5696353336845714E-2</v>
       </c>
-      <c r="I59">
-        <f t="shared" si="1"/>
+      <c r="J59">
+        <f>I59+$M$8*SIN(F59-H59)</f>
         <v>2.4269839605142854E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>0.96699999999999997</v>
       </c>
@@ -9218,18 +9456,22 @@
         <v>-5.7910950129274184E-2</v>
       </c>
       <c r="G60">
+        <f>DEGREES(F60)</f>
+        <v>-3.3180530299999997</v>
+      </c>
+      <c r="H60">
         <v>-7.9609325656500085E-2</v>
       </c>
-      <c r="H60">
-        <f t="shared" si="0"/>
+      <c r="I60">
+        <f>B60-$M$6*COS(C60+D60)-$M$7*COS(C60+D60+E60)-$M$10</f>
         <v>1.3615659272167902E-2</v>
       </c>
-      <c r="I60">
-        <f t="shared" si="1"/>
+      <c r="J60">
+        <f>I60+$M$8*SIN(F60-H60)</f>
         <v>1.7627990497836494E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>0.98299999999999998</v>
       </c>
@@ -9249,18 +9491,22 @@
         <v>-4.516427077162196E-2</v>
       </c>
       <c r="G61">
+        <f>DEGREES(F61)</f>
+        <v>-2.5877221000000001</v>
+      </c>
+      <c r="H61">
         <v>-5.0262598649913663E-2</v>
       </c>
-      <c r="H61">
-        <f t="shared" si="0"/>
+      <c r="I61">
+        <f>B61-$M$6*COS(C61+D61)-$M$7*COS(C61+D61+E61)-$M$10</f>
         <v>1.126199794818572E-2</v>
       </c>
-      <c r="I61">
-        <f t="shared" si="1"/>
+      <c r="J61">
+        <f>I61+$M$8*SIN(F61-H61)</f>
         <v>1.2204819532953007E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>0.99999999999999989</v>
       </c>
@@ -9280,18 +9526,22 @@
         <v>-2.8714690924561824E-2</v>
       </c>
       <c r="G62">
+        <f>DEGREES(F62)</f>
+        <v>-1.6452306000000003</v>
+      </c>
+      <c r="H62">
         <v>-2.3497319024913518E-2</v>
       </c>
-      <c r="H62">
-        <f t="shared" si="0"/>
+      <c r="I62">
+        <f>B62-$M$6*COS(C62+D62)-$M$7*COS(C62+D62+E62)-$M$10</f>
         <v>9.1062699711585982E-3</v>
       </c>
-      <c r="I62">
-        <f t="shared" si="1"/>
+      <c r="J62">
+        <f>I62+$M$8*SIN(F62-H62)</f>
         <v>8.1414340576219466E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1.0169999999999999</v>
       </c>
@@ -9311,18 +9561,22 @@
         <v>-1.3497230102671435E-2</v>
       </c>
       <c r="G63">
+        <f>DEGREES(F63)</f>
+        <v>-0.77333432000000002</v>
+      </c>
+      <c r="H63">
         <v>-3.0530370908045568E-3</v>
       </c>
-      <c r="H63">
-        <f t="shared" si="0"/>
+      <c r="I63">
+        <f>B63-$M$6*COS(C63+D63)-$M$7*COS(C63+D63+E63)-$M$10</f>
         <v>6.9456642771068555E-3</v>
       </c>
-      <c r="I63">
-        <f t="shared" si="1"/>
+      <c r="J63">
+        <f>I63+$M$8*SIN(F63-H63)</f>
         <v>5.0142713811033596E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1.0329999999999999</v>
       </c>
@@ -9342,18 +9596,22 @@
         <v>3.9026155486538881E-4</v>
       </c>
       <c r="G64">
+        <f>DEGREES(F64)</f>
+        <v>2.2360339999999996E-2</v>
+      </c>
+      <c r="H64">
         <v>1.3483288063540655E-2</v>
       </c>
-      <c r="H64">
-        <f t="shared" si="0"/>
+      <c r="I64">
+        <f>B64-$M$6*COS(C64+D64)-$M$7*COS(C64+D64+E64)-$M$10</f>
         <v>4.8394325101331903E-3</v>
       </c>
-      <c r="I64">
-        <f t="shared" si="1"/>
+      <c r="J64">
+        <f>I64+$M$8*SIN(F64-H64)</f>
         <v>2.418229111251901E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1.0499999999999998</v>
       </c>
@@ -9373,18 +9631,22 @@
         <v>1.3981842411570385E-2</v>
       </c>
       <c r="G65">
+        <f>DEGREES(F65)</f>
+        <v>0.80110055999999996</v>
+      </c>
+      <c r="H65">
         <v>2.9139152729718763E-2</v>
       </c>
-      <c r="H65">
-        <f t="shared" si="0"/>
+      <c r="I65">
+        <f>B65-$M$6*COS(C65+D65)-$M$7*COS(C65+D65+E65)-$M$10</f>
         <v>3.39473300210269E-3</v>
       </c>
-      <c r="I65">
-        <f t="shared" si="1"/>
+      <c r="J65">
+        <f>I65+$M$8*SIN(F65-H65)</f>
         <v>5.9182303019204331E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1.0670000000000002</v>
       </c>
@@ -9404,18 +9666,22 @@
         <v>2.6364026684637346E-2</v>
       </c>
       <c r="G66">
+        <f>DEGREES(F66)</f>
+        <v>1.5105474600000002</v>
+      </c>
+      <c r="H66">
         <v>4.3961480084669789E-2</v>
       </c>
-      <c r="H66">
-        <f t="shared" si="0"/>
+      <c r="I66">
+        <f>B66-$M$6*COS(C66+D66)-$M$7*COS(C66+D66+E66)-$M$10</f>
         <v>2.6195836683922114E-3</v>
       </c>
-      <c r="I66">
-        <f t="shared" si="1"/>
+      <c r="J66">
+        <f>I66+$M$8*SIN(F66-H66)</f>
         <v>-6.3451745666704383E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1.0830000000000002</v>
       </c>
@@ -9435,18 +9701,22 @@
         <v>3.4775942956584607E-2</v>
       </c>
       <c r="G67">
+        <f>DEGREES(F67)</f>
+        <v>1.9925147599999999</v>
+      </c>
+      <c r="H67">
         <v>5.4385462707397393E-2</v>
       </c>
-      <c r="H67">
-        <f t="shared" ref="H67:H74" si="2">B67-$L$6*COS(C67+D67)-$L$7*COS(C67+D67+E67)-$L$10</f>
+      <c r="I67">
+        <f>B67-$M$6*COS(C67+D67)-$M$7*COS(C67+D67+E67)-$M$10</f>
         <v>2.0220618820427916E-3</v>
       </c>
-      <c r="I67">
-        <f t="shared" ref="I67:I74" si="3">H67+$L$8*SIN(F67-G67)</f>
+      <c r="J67">
+        <f>I67+$M$8*SIN(F67-H67)</f>
         <v>-1.6040630256394049E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1.1000000000000001</v>
       </c>
@@ -9466,18 +9736,22 @@
         <v>4.4529557005458839E-2</v>
       </c>
       <c r="G68">
+        <f>DEGREES(F68)</f>
+        <v>2.5513556799999999</v>
+      </c>
+      <c r="H68">
         <v>6.6492597925648669E-2</v>
       </c>
-      <c r="H68">
-        <f t="shared" si="2"/>
+      <c r="I68">
+        <f>B68-$M$6*COS(C68+D68)-$M$7*COS(C68+D68+E68)-$M$10</f>
         <v>1.6709306523434719E-3</v>
       </c>
-      <c r="I68">
-        <f t="shared" si="3"/>
+      <c r="J68">
+        <f>I68+$M$8*SIN(F68-H68)</f>
         <v>-2.3903330611051215E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1.117</v>
       </c>
@@ -9497,18 +9771,22 @@
         <v>5.1917153676577579E-2</v>
       </c>
       <c r="G69">
+        <f>DEGREES(F69)</f>
+        <v>2.9746337900000004</v>
+      </c>
+      <c r="H69">
         <v>7.5692986758470748E-2</v>
       </c>
-      <c r="H69">
-        <f t="shared" si="2"/>
+      <c r="I69">
+        <f>B69-$M$6*COS(C69+D69)-$M$7*COS(C69+D69+E69)-$M$10</f>
         <v>1.3549758566331338E-3</v>
       </c>
-      <c r="I69">
-        <f t="shared" si="3"/>
+      <c r="J69">
+        <f>I69+$M$8*SIN(F69-H69)</f>
         <v>-3.0414369209552277E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1.133</v>
       </c>
@@ -9528,18 +9806,22 @@
         <v>5.8089555605750222E-2</v>
       </c>
       <c r="G70">
+        <f>DEGREES(F70)</f>
+        <v>3.3282863699999998</v>
+      </c>
+      <c r="H70">
         <v>8.359138475298046E-2</v>
       </c>
-      <c r="H70">
-        <f t="shared" si="2"/>
+      <c r="I70">
+        <f>B70-$M$6*COS(C70+D70)-$M$7*COS(C70+D70+E70)-$M$10</f>
         <v>1.0495893530064748E-3</v>
       </c>
-      <c r="I70">
-        <f t="shared" si="3"/>
+      <c r="J70">
+        <f>I70+$M$8*SIN(F70-H70)</f>
         <v>-3.6659122139036798E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1.1499999999999999</v>
       </c>
@@ -9559,18 +9841,22 @@
         <v>6.5271836106987474E-2</v>
       </c>
       <c r="G71">
+        <f>DEGREES(F71)</f>
+        <v>3.7398007299999998</v>
+      </c>
+      <c r="H71">
         <v>9.265304242501636E-2</v>
       </c>
-      <c r="H71">
-        <f t="shared" si="2"/>
+      <c r="I71">
+        <f>B71-$M$6*COS(C71+D71)-$M$7*COS(C71+D71+E71)-$M$10</f>
         <v>4.2587856066123031E-4</v>
       </c>
-      <c r="I71">
-        <f t="shared" si="3"/>
+      <c r="J71">
+        <f>I71+$M$8*SIN(F71-H71)</f>
         <v>-4.6370516990230336E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1.1669999999999998</v>
       </c>
@@ -9590,18 +9876,22 @@
         <v>7.2909759418600312E-2</v>
       </c>
       <c r="G72">
+        <f>DEGREES(F72)</f>
+        <v>4.1774215000000003</v>
+      </c>
+      <c r="H72">
         <v>0.10165873087859929</v>
       </c>
-      <c r="H72">
-        <f t="shared" si="2"/>
+      <c r="I72">
+        <f>B72-$M$6*COS(C72+D72)-$M$7*COS(C72+D72+E72)-$M$10</f>
         <v>3.872033836704869E-4</v>
       </c>
-      <c r="I72">
-        <f t="shared" si="3"/>
+      <c r="J72">
+        <f>I72+$M$8*SIN(F72-H72)</f>
         <v>-4.9285658826225811E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1.1829999999999998</v>
       </c>
@@ -9621,18 +9911,22 @@
         <v>8.158134246053371E-2</v>
       </c>
       <c r="G73">
+        <f>DEGREES(F73)</f>
+        <v>4.6742666100000001</v>
+      </c>
+      <c r="H73">
         <v>0.1118953387925571</v>
       </c>
-      <c r="H73">
-        <f t="shared" si="2"/>
+      <c r="I73">
+        <f>B73-$M$6*COS(C73+D73)-$M$7*COS(C73+D73+E73)-$M$10</f>
         <v>2.1299940437380371E-4</v>
       </c>
-      <c r="I73">
-        <f t="shared" si="3"/>
+      <c r="J73">
+        <f>I73+$M$8*SIN(F73-H73)</f>
         <v>-5.3920612013170213E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1.2000000000000002</v>
       </c>
@@ -9652,14 +9946,18 @@
         <v>8.8410776902745195E-2</v>
       </c>
       <c r="G74">
+        <f>DEGREES(F74)</f>
+        <v>5.0655643799999996</v>
+      </c>
+      <c r="H74">
         <v>0.1199987869687703</v>
       </c>
-      <c r="H74">
-        <f t="shared" si="2"/>
+      <c r="I74">
+        <f>B74-$M$6*COS(C74+D74)-$M$7*COS(C74+D74+E74)-$M$10</f>
         <v>0</v>
       </c>
-      <c r="I74">
-        <f t="shared" si="3"/>
+      <c r="J74">
+        <f>I74+$M$8*SIN(F74-H74)</f>
         <v>-5.840549084311481E-3</v>
       </c>
     </row>

</xml_diff>